<commit_message>
finish module jenis pengadaan dan form pemetaan
</commit_message>
<xml_diff>
--- a/assets/data/SITARING HAJA KIRIM ok.xlsx
+++ b/assets/data/SITARING HAJA KIRIM ok.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21601"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\sitaring\assets\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3900A2B8-7CAC-4195-BC8E-52B9D6E3E6BF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="9495" windowHeight="4635" tabRatio="810"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mei" sheetId="14" r:id="rId1"/>
@@ -22,7 +28,14 @@
     <definedName name="sum_rincian">'[1]DATA PENGADAAN'!$L$9:$L$1048576</definedName>
     <definedName name="sum_sp2d">'[1]DATA SP2D'!$E$7:$E$1048576</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -813,13 +826,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2204,6 +2217,33 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2213,13 +2253,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2246,82 +2334,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="37" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="34" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2339,12 +2397,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2363,49 +2415,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2413,14 +2426,14 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="5"/>
-    <cellStyle name="Normal 2 4" xfId="6"/>
-    <cellStyle name="Normal 2 4 2" xfId="7"/>
-    <cellStyle name="Normal 2 4 3" xfId="3"/>
-    <cellStyle name="Normal 2 4 3 2" xfId="8"/>
-    <cellStyle name="Normal 2 57 5" xfId="9"/>
-    <cellStyle name="Normal 2 58 2 2 3 2 2 2 2" xfId="10"/>
-    <cellStyle name="Normal_lapdik bulanan diknas Juli-Agustuz" xfId="4"/>
+    <cellStyle name="Normal 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 2 4" xfId="6" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 2 4 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 2 4 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 2 4 3 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 2 57 5" xfId="9" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Normal 2 58 2 2 3 2 2 2 2" xfId="10" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Normal_lapdik bulanan diknas Juli-Agustuz" xfId="4" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -3431,7 +3444,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3464,9 +3477,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3499,6 +3529,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3674,16 +3721,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:W213"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="69" workbookViewId="0">
-      <pane ySplit="2175" topLeftCell="A46" activePane="bottomLeft"/>
+      <pane ySplit="2175" topLeftCell="A13" activePane="bottomLeft"/>
       <selection activeCell="F5" sqref="F5:G8"/>
-      <selection pane="bottomLeft" activeCell="I188" sqref="I188:K188"/>
+      <selection pane="bottomLeft" activeCell="N41" sqref="N41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.42578125" customWidth="1"/>
     <col min="2" max="2" width="26" style="200" customWidth="1"/>
@@ -3709,88 +3759,88 @@
     <col min="23" max="23" width="28.28515625" style="68" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="23.25">
-      <c r="A1" s="290" t="s">
+    <row r="1" spans="1:23" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="256" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="290"/>
-      <c r="C1" s="290"/>
-      <c r="D1" s="290"/>
-      <c r="E1" s="290"/>
-      <c r="F1" s="290"/>
-      <c r="G1" s="290"/>
-      <c r="H1" s="290"/>
-      <c r="I1" s="290"/>
-      <c r="J1" s="290"/>
-      <c r="K1" s="290"/>
-      <c r="L1" s="290"/>
-      <c r="M1" s="290"/>
-      <c r="N1" s="290"/>
-      <c r="O1" s="290"/>
-      <c r="P1" s="290"/>
-      <c r="Q1" s="290"/>
-      <c r="R1" s="290"/>
-      <c r="S1" s="290"/>
-      <c r="T1" s="290"/>
-      <c r="U1" s="290"/>
-      <c r="V1" s="290"/>
-      <c r="W1" s="290"/>
-    </row>
-    <row r="2" spans="1:23" ht="18.75">
-      <c r="A2" s="291" t="s">
+      <c r="B1" s="256"/>
+      <c r="C1" s="256"/>
+      <c r="D1" s="256"/>
+      <c r="E1" s="256"/>
+      <c r="F1" s="256"/>
+      <c r="G1" s="256"/>
+      <c r="H1" s="256"/>
+      <c r="I1" s="256"/>
+      <c r="J1" s="256"/>
+      <c r="K1" s="256"/>
+      <c r="L1" s="256"/>
+      <c r="M1" s="256"/>
+      <c r="N1" s="256"/>
+      <c r="O1" s="256"/>
+      <c r="P1" s="256"/>
+      <c r="Q1" s="256"/>
+      <c r="R1" s="256"/>
+      <c r="S1" s="256"/>
+      <c r="T1" s="256"/>
+      <c r="U1" s="256"/>
+      <c r="V1" s="256"/>
+      <c r="W1" s="256"/>
+    </row>
+    <row r="2" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="257" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="291"/>
-      <c r="C2" s="291"/>
-      <c r="D2" s="291"/>
-      <c r="E2" s="291"/>
-      <c r="F2" s="291"/>
-      <c r="G2" s="291"/>
-      <c r="H2" s="291"/>
-      <c r="I2" s="291"/>
-      <c r="J2" s="291"/>
-      <c r="K2" s="291"/>
-      <c r="L2" s="291"/>
-      <c r="M2" s="291"/>
-      <c r="N2" s="291"/>
-      <c r="O2" s="291"/>
-      <c r="P2" s="291"/>
-      <c r="Q2" s="291"/>
-      <c r="R2" s="291"/>
-      <c r="S2" s="291"/>
-      <c r="T2" s="291"/>
-      <c r="U2" s="291"/>
-      <c r="V2" s="291"/>
-      <c r="W2" s="291"/>
-    </row>
-    <row r="3" spans="1:23" ht="18.75">
-      <c r="A3" s="291" t="s">
+      <c r="B2" s="257"/>
+      <c r="C2" s="257"/>
+      <c r="D2" s="257"/>
+      <c r="E2" s="257"/>
+      <c r="F2" s="257"/>
+      <c r="G2" s="257"/>
+      <c r="H2" s="257"/>
+      <c r="I2" s="257"/>
+      <c r="J2" s="257"/>
+      <c r="K2" s="257"/>
+      <c r="L2" s="257"/>
+      <c r="M2" s="257"/>
+      <c r="N2" s="257"/>
+      <c r="O2" s="257"/>
+      <c r="P2" s="257"/>
+      <c r="Q2" s="257"/>
+      <c r="R2" s="257"/>
+      <c r="S2" s="257"/>
+      <c r="T2" s="257"/>
+      <c r="U2" s="257"/>
+      <c r="V2" s="257"/>
+      <c r="W2" s="257"/>
+    </row>
+    <row r="3" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="257" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="291"/>
-      <c r="C3" s="291"/>
-      <c r="D3" s="291"/>
-      <c r="E3" s="291"/>
-      <c r="F3" s="291"/>
-      <c r="G3" s="291"/>
-      <c r="H3" s="291"/>
-      <c r="I3" s="291"/>
-      <c r="J3" s="291"/>
-      <c r="K3" s="291"/>
-      <c r="L3" s="291"/>
-      <c r="M3" s="291"/>
-      <c r="N3" s="291"/>
-      <c r="O3" s="291"/>
-      <c r="P3" s="291"/>
-      <c r="Q3" s="291"/>
-      <c r="R3" s="291"/>
-      <c r="S3" s="291"/>
-      <c r="T3" s="291"/>
-      <c r="U3" s="291"/>
-      <c r="V3" s="291"/>
-      <c r="W3" s="291"/>
-    </row>
-    <row r="4" spans="1:23">
+      <c r="B3" s="257"/>
+      <c r="C3" s="257"/>
+      <c r="D3" s="257"/>
+      <c r="E3" s="257"/>
+      <c r="F3" s="257"/>
+      <c r="G3" s="257"/>
+      <c r="H3" s="257"/>
+      <c r="I3" s="257"/>
+      <c r="J3" s="257"/>
+      <c r="K3" s="257"/>
+      <c r="L3" s="257"/>
+      <c r="M3" s="257"/>
+      <c r="N3" s="257"/>
+      <c r="O3" s="257"/>
+      <c r="P3" s="257"/>
+      <c r="Q3" s="257"/>
+      <c r="R3" s="257"/>
+      <c r="S3" s="257"/>
+      <c r="T3" s="257"/>
+      <c r="U3" s="257"/>
+      <c r="V3" s="257"/>
+      <c r="W3" s="257"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="E4" s="62"/>
       <c r="I4" s="59"/>
       <c r="J4" s="59"/>
@@ -3801,97 +3851,97 @@
       <c r="S4" s="58"/>
       <c r="T4" s="67"/>
     </row>
-    <row r="5" spans="1:23" ht="15" customHeight="1">
-      <c r="A5" s="253" t="s">
+    <row r="5" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="262" t="s">
         <v>239</v>
       </c>
-      <c r="B5" s="253" t="s">
+      <c r="B5" s="262" t="s">
         <v>238</v>
       </c>
-      <c r="C5" s="283" t="s">
+      <c r="C5" s="265" t="s">
         <v>240</v>
       </c>
-      <c r="D5" s="253" t="s">
+      <c r="D5" s="262" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="256" t="s">
+      <c r="E5" s="258" t="s">
         <v>241</v>
       </c>
-      <c r="F5" s="259" t="s">
+      <c r="F5" s="284" t="s">
         <v>40</v>
       </c>
-      <c r="G5" s="260"/>
-      <c r="H5" s="256" t="s">
+      <c r="G5" s="285"/>
+      <c r="H5" s="258" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="265" t="s">
+      <c r="I5" s="290" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="265"/>
-      <c r="K5" s="265"/>
-      <c r="L5" s="265"/>
-      <c r="M5" s="265"/>
-      <c r="N5" s="256" t="s">
+      <c r="J5" s="290"/>
+      <c r="K5" s="290"/>
+      <c r="L5" s="290"/>
+      <c r="M5" s="290"/>
+      <c r="N5" s="258" t="s">
         <v>27</v>
       </c>
-      <c r="O5" s="256" t="s">
+      <c r="O5" s="258" t="s">
         <v>26</v>
       </c>
-      <c r="P5" s="253" t="s">
+      <c r="P5" s="262" t="s">
         <v>9</v>
       </c>
-      <c r="Q5" s="253" t="s">
+      <c r="Q5" s="262" t="s">
         <v>243</v>
       </c>
-      <c r="R5" s="292" t="s">
+      <c r="R5" s="261" t="s">
         <v>31</v>
       </c>
-      <c r="S5" s="292"/>
-      <c r="T5" s="292"/>
-      <c r="U5" s="256" t="s">
+      <c r="S5" s="261"/>
+      <c r="T5" s="261"/>
+      <c r="U5" s="258" t="s">
         <v>29</v>
       </c>
-      <c r="V5" s="287" t="s">
+      <c r="V5" s="253" t="s">
         <v>30</v>
       </c>
-      <c r="W5" s="287" t="s">
+      <c r="W5" s="253" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="15" customHeight="1">
-      <c r="A6" s="254"/>
-      <c r="B6" s="254"/>
-      <c r="C6" s="284"/>
-      <c r="D6" s="254"/>
-      <c r="E6" s="257"/>
-      <c r="F6" s="261"/>
-      <c r="G6" s="262"/>
-      <c r="H6" s="257"/>
-      <c r="I6" s="266"/>
-      <c r="J6" s="266"/>
-      <c r="K6" s="266"/>
-      <c r="L6" s="266"/>
-      <c r="M6" s="266"/>
-      <c r="N6" s="257"/>
-      <c r="O6" s="257"/>
-      <c r="P6" s="254"/>
-      <c r="Q6" s="254"/>
-      <c r="R6" s="292"/>
-      <c r="S6" s="292"/>
-      <c r="T6" s="292"/>
-      <c r="U6" s="257"/>
-      <c r="V6" s="288"/>
-      <c r="W6" s="288"/>
-    </row>
-    <row r="7" spans="1:23" ht="15" customHeight="1">
-      <c r="A7" s="254"/>
-      <c r="B7" s="254"/>
-      <c r="C7" s="284"/>
-      <c r="D7" s="254"/>
-      <c r="E7" s="257"/>
-      <c r="F7" s="261"/>
-      <c r="G7" s="262"/>
-      <c r="H7" s="257"/>
+    <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="263"/>
+      <c r="B6" s="263"/>
+      <c r="C6" s="266"/>
+      <c r="D6" s="263"/>
+      <c r="E6" s="259"/>
+      <c r="F6" s="286"/>
+      <c r="G6" s="287"/>
+      <c r="H6" s="259"/>
+      <c r="I6" s="291"/>
+      <c r="J6" s="291"/>
+      <c r="K6" s="291"/>
+      <c r="L6" s="291"/>
+      <c r="M6" s="291"/>
+      <c r="N6" s="259"/>
+      <c r="O6" s="259"/>
+      <c r="P6" s="263"/>
+      <c r="Q6" s="263"/>
+      <c r="R6" s="261"/>
+      <c r="S6" s="261"/>
+      <c r="T6" s="261"/>
+      <c r="U6" s="259"/>
+      <c r="V6" s="254"/>
+      <c r="W6" s="254"/>
+    </row>
+    <row r="7" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="263"/>
+      <c r="B7" s="263"/>
+      <c r="C7" s="266"/>
+      <c r="D7" s="263"/>
+      <c r="E7" s="259"/>
+      <c r="F7" s="286"/>
+      <c r="G7" s="287"/>
+      <c r="H7" s="259"/>
       <c r="I7" s="203" t="s">
         <v>242</v>
       </c>
@@ -3901,36 +3951,36 @@
       <c r="K7" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="256" t="s">
+      <c r="L7" s="258" t="s">
         <v>4</v>
       </c>
-      <c r="M7" s="272" t="s">
+      <c r="M7" s="282" t="s">
         <v>36</v>
       </c>
-      <c r="N7" s="257"/>
-      <c r="O7" s="257"/>
-      <c r="P7" s="254"/>
-      <c r="Q7" s="255"/>
-      <c r="R7" s="286" t="s">
+      <c r="N7" s="259"/>
+      <c r="O7" s="259"/>
+      <c r="P7" s="263"/>
+      <c r="Q7" s="264"/>
+      <c r="R7" s="292" t="s">
         <v>32</v>
       </c>
-      <c r="S7" s="286"/>
+      <c r="S7" s="292"/>
       <c r="T7" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="U7" s="257"/>
-      <c r="V7" s="288"/>
-      <c r="W7" s="288"/>
-    </row>
-    <row r="8" spans="1:23">
-      <c r="A8" s="255"/>
-      <c r="B8" s="255"/>
-      <c r="C8" s="285"/>
-      <c r="D8" s="255"/>
-      <c r="E8" s="258"/>
-      <c r="F8" s="263"/>
-      <c r="G8" s="264"/>
-      <c r="H8" s="258"/>
+      <c r="U7" s="259"/>
+      <c r="V7" s="254"/>
+      <c r="W7" s="254"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" s="264"/>
+      <c r="B8" s="264"/>
+      <c r="C8" s="267"/>
+      <c r="D8" s="264"/>
+      <c r="E8" s="260"/>
+      <c r="F8" s="288"/>
+      <c r="G8" s="289"/>
+      <c r="H8" s="260"/>
       <c r="I8" s="249" t="s">
         <v>5</v>
       </c>
@@ -3940,11 +3990,11 @@
       <c r="K8" s="247" t="s">
         <v>5</v>
       </c>
-      <c r="L8" s="258"/>
-      <c r="M8" s="273"/>
-      <c r="N8" s="258"/>
-      <c r="O8" s="258"/>
-      <c r="P8" s="255"/>
+      <c r="L8" s="260"/>
+      <c r="M8" s="283"/>
+      <c r="N8" s="260"/>
+      <c r="O8" s="260"/>
+      <c r="P8" s="264"/>
       <c r="Q8" s="75" t="s">
         <v>34</v>
       </c>
@@ -3957,11 +4007,11 @@
       <c r="T8" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="U8" s="258"/>
-      <c r="V8" s="289"/>
-      <c r="W8" s="289"/>
-    </row>
-    <row r="9" spans="1:23">
+      <c r="U8" s="260"/>
+      <c r="V8" s="255"/>
+      <c r="W8" s="255"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="81">
         <v>1</v>
       </c>
@@ -3977,10 +4027,10 @@
       <c r="E9" s="81">
         <v>5</v>
       </c>
-      <c r="F9" s="270">
+      <c r="F9" s="280">
         <v>6</v>
       </c>
-      <c r="G9" s="271"/>
+      <c r="G9" s="281"/>
       <c r="H9" s="75">
         <v>7</v>
       </c>
@@ -4030,7 +4080,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="80"/>
       <c r="B10" s="223"/>
       <c r="C10" s="83"/>
@@ -4055,7 +4105,7 @@
       <c r="V10" s="86"/>
       <c r="W10" s="86"/>
     </row>
-    <row r="11" spans="1:23">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="80"/>
       <c r="B11" s="223"/>
       <c r="C11" s="83"/>
@@ -4080,7 +4130,7 @@
       <c r="V11" s="86"/>
       <c r="W11" s="86"/>
     </row>
-    <row r="12" spans="1:23" s="97" customFormat="1">
+    <row r="12" spans="1:23" s="97" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="87">
         <f>MAX(A14:A190)</f>
         <v>134</v>
@@ -4120,7 +4170,7 @@
       <c r="V12" s="96"/>
       <c r="W12" s="96"/>
     </row>
-    <row r="13" spans="1:23">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="98"/>
       <c r="B13" s="225"/>
       <c r="C13" s="208"/>
@@ -4145,7 +4195,7 @@
       <c r="V13" s="104"/>
       <c r="W13" s="104"/>
     </row>
-    <row r="14" spans="1:23" s="115" customFormat="1" ht="33" customHeight="1">
+    <row r="14" spans="1:23" s="115" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="105"/>
       <c r="B14" s="226" t="s">
         <v>44</v>
@@ -4188,7 +4238,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:23" s="127" customFormat="1" ht="36" customHeight="1">
+    <row r="15" spans="1:23" s="127" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="116"/>
       <c r="B15" s="227" t="s">
         <v>46</v>
@@ -4229,7 +4279,7 @@
       <c r="V15" s="126"/>
       <c r="W15" s="135"/>
     </row>
-    <row r="16" spans="1:23" s="127" customFormat="1" ht="83.25" customHeight="1">
+    <row r="16" spans="1:23" s="127" customFormat="1" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="128">
         <v>1</v>
       </c>
@@ -4271,7 +4321,7 @@
       </c>
       <c r="W16" s="135"/>
     </row>
-    <row r="17" spans="1:23" s="143" customFormat="1">
+    <row r="17" spans="1:23" s="143" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="128"/>
       <c r="B17" s="136"/>
       <c r="C17" s="142"/>
@@ -4296,7 +4346,7 @@
       <c r="V17" s="126"/>
       <c r="W17" s="126"/>
     </row>
-    <row r="18" spans="1:23" s="154" customFormat="1" ht="33" customHeight="1">
+    <row r="18" spans="1:23" s="154" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="144"/>
       <c r="B18" s="228" t="s">
         <v>52</v>
@@ -4339,7 +4389,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:23" s="127" customFormat="1" ht="30" customHeight="1">
+    <row r="19" spans="1:23" s="127" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="116"/>
       <c r="B19" s="227" t="s">
         <v>54</v>
@@ -4380,7 +4430,7 @@
       <c r="V19" s="126"/>
       <c r="W19" s="135"/>
     </row>
-    <row r="20" spans="1:23" s="127" customFormat="1" ht="48.75" customHeight="1">
+    <row r="20" spans="1:23" s="127" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="116">
         <v>2</v>
       </c>
@@ -4434,7 +4484,7 @@
       <c r="V20" s="126"/>
       <c r="W20" s="135"/>
     </row>
-    <row r="21" spans="1:23" s="127" customFormat="1" ht="48.75" customHeight="1">
+    <row r="21" spans="1:23" s="127" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="116">
         <v>3</v>
       </c>
@@ -4488,7 +4538,7 @@
       <c r="V21" s="126"/>
       <c r="W21" s="135"/>
     </row>
-    <row r="22" spans="1:23" s="127" customFormat="1">
+    <row r="22" spans="1:23" s="127" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="116"/>
       <c r="B22" s="227"/>
       <c r="C22" s="142"/>
@@ -4513,7 +4563,7 @@
       <c r="V22" s="126"/>
       <c r="W22" s="126"/>
     </row>
-    <row r="23" spans="1:23" s="154" customFormat="1" ht="62.25" customHeight="1">
+    <row r="23" spans="1:23" s="154" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="144"/>
       <c r="B23" s="230" t="s">
         <v>63</v>
@@ -4556,7 +4606,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="24" spans="1:23" s="127" customFormat="1" ht="49.5" customHeight="1">
+    <row r="24" spans="1:23" s="127" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="116"/>
       <c r="B24" s="231" t="s">
         <v>65</v>
@@ -4597,7 +4647,7 @@
       <c r="V24" s="135"/>
       <c r="W24" s="135"/>
     </row>
-    <row r="25" spans="1:23" s="127" customFormat="1" ht="58.5" customHeight="1">
+    <row r="25" spans="1:23" s="127" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="116">
         <v>4</v>
       </c>
@@ -4631,13 +4681,13 @@
         <v>0</v>
       </c>
       <c r="T25" s="133"/>
-      <c r="U25" s="267" t="s">
+      <c r="U25" s="271" t="s">
         <v>68</v>
       </c>
       <c r="V25" s="160"/>
       <c r="W25" s="160"/>
     </row>
-    <row r="26" spans="1:23" s="127" customFormat="1" ht="45" customHeight="1">
+    <row r="26" spans="1:23" s="127" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="116">
         <v>5</v>
       </c>
@@ -4687,13 +4737,13 @@
       <c r="T26" s="133">
         <v>100</v>
       </c>
-      <c r="U26" s="268"/>
+      <c r="U26" s="272"/>
       <c r="V26" s="160" t="s">
         <v>73</v>
       </c>
       <c r="W26" s="160"/>
     </row>
-    <row r="27" spans="1:23" s="127" customFormat="1" ht="50.25" customHeight="1">
+    <row r="27" spans="1:23" s="127" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="116">
         <v>6</v>
       </c>
@@ -4727,11 +4777,11 @@
         <v>0</v>
       </c>
       <c r="T27" s="133"/>
-      <c r="U27" s="269"/>
+      <c r="U27" s="273"/>
       <c r="V27" s="126"/>
       <c r="W27" s="126"/>
     </row>
-    <row r="28" spans="1:23" s="127" customFormat="1">
+    <row r="28" spans="1:23" s="127" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="116"/>
       <c r="B28" s="227"/>
       <c r="C28" s="142"/>
@@ -4756,7 +4806,7 @@
       <c r="V28" s="126"/>
       <c r="W28" s="126"/>
     </row>
-    <row r="29" spans="1:23" s="154" customFormat="1" ht="68.25" customHeight="1">
+    <row r="29" spans="1:23" s="154" customFormat="1" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="161"/>
       <c r="B29" s="230" t="s">
         <v>75</v>
@@ -4799,7 +4849,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="30" spans="1:23" s="127" customFormat="1" ht="42.75" customHeight="1">
+    <row r="30" spans="1:23" s="127" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="116"/>
       <c r="B30" s="231" t="s">
         <v>77</v>
@@ -4840,7 +4890,7 @@
       <c r="V30" s="135"/>
       <c r="W30" s="135"/>
     </row>
-    <row r="31" spans="1:23" s="127" customFormat="1" ht="69" customHeight="1">
+    <row r="31" spans="1:23" s="127" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="116">
         <v>7</v>
       </c>
@@ -4874,13 +4924,13 @@
         <v>0</v>
       </c>
       <c r="T31" s="133"/>
-      <c r="U31" s="267" t="s">
+      <c r="U31" s="271" t="s">
         <v>80</v>
       </c>
       <c r="V31" s="126"/>
       <c r="W31" s="126"/>
     </row>
-    <row r="32" spans="1:23" s="127" customFormat="1" ht="45.75" customHeight="1">
+    <row r="32" spans="1:23" s="127" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="116">
         <v>8</v>
       </c>
@@ -4930,13 +4980,13 @@
       <c r="T32" s="133">
         <v>100</v>
       </c>
-      <c r="U32" s="268"/>
+      <c r="U32" s="272"/>
       <c r="V32" s="160" t="s">
         <v>83</v>
       </c>
       <c r="W32" s="160"/>
     </row>
-    <row r="33" spans="1:23" s="127" customFormat="1" ht="44.25" customHeight="1">
+    <row r="33" spans="1:23" s="127" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="116">
         <v>9</v>
       </c>
@@ -4970,11 +5020,11 @@
         <v>0</v>
       </c>
       <c r="T33" s="133"/>
-      <c r="U33" s="269"/>
+      <c r="U33" s="273"/>
       <c r="V33" s="126"/>
       <c r="W33" s="126"/>
     </row>
-    <row r="34" spans="1:23" s="127" customFormat="1" ht="58.5" customHeight="1">
+    <row r="34" spans="1:23" s="127" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="116">
         <v>10</v>
       </c>
@@ -5008,13 +5058,13 @@
         <v>0</v>
       </c>
       <c r="T34" s="133"/>
-      <c r="U34" s="267" t="s">
+      <c r="U34" s="271" t="s">
         <v>85</v>
       </c>
       <c r="V34" s="126"/>
       <c r="W34" s="126"/>
     </row>
-    <row r="35" spans="1:23" s="127" customFormat="1" ht="45" customHeight="1">
+    <row r="35" spans="1:23" s="127" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="116">
         <v>11</v>
       </c>
@@ -5064,13 +5114,13 @@
       <c r="T35" s="133">
         <v>100</v>
       </c>
-      <c r="U35" s="268"/>
+      <c r="U35" s="272"/>
       <c r="V35" s="160" t="s">
         <v>86</v>
       </c>
       <c r="W35" s="160"/>
     </row>
-    <row r="36" spans="1:23" s="127" customFormat="1" ht="45.75" customHeight="1">
+    <row r="36" spans="1:23" s="127" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="116">
         <v>12</v>
       </c>
@@ -5104,11 +5154,11 @@
         <v>0</v>
       </c>
       <c r="T36" s="133"/>
-      <c r="U36" s="269"/>
+      <c r="U36" s="273"/>
       <c r="V36" s="126"/>
       <c r="W36" s="126"/>
     </row>
-    <row r="37" spans="1:23" s="127" customFormat="1" ht="53.25" customHeight="1">
+    <row r="37" spans="1:23" s="127" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="116">
         <v>13</v>
       </c>
@@ -5142,13 +5192,13 @@
         <v>0</v>
       </c>
       <c r="T37" s="133"/>
-      <c r="U37" s="267" t="s">
+      <c r="U37" s="271" t="s">
         <v>88</v>
       </c>
       <c r="V37" s="135"/>
       <c r="W37" s="135"/>
     </row>
-    <row r="38" spans="1:23" s="127" customFormat="1" ht="45.75" customHeight="1">
+    <row r="38" spans="1:23" s="127" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="116">
         <v>14</v>
       </c>
@@ -5198,13 +5248,13 @@
       <c r="T38" s="133">
         <v>100</v>
       </c>
-      <c r="U38" s="268"/>
+      <c r="U38" s="272"/>
       <c r="V38" s="160" t="s">
         <v>89</v>
       </c>
       <c r="W38" s="160"/>
     </row>
-    <row r="39" spans="1:23" s="127" customFormat="1" ht="42.75" customHeight="1">
+    <row r="39" spans="1:23" s="127" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="116">
         <v>15</v>
       </c>
@@ -5238,11 +5288,11 @@
         <v>0</v>
       </c>
       <c r="T39" s="133"/>
-      <c r="U39" s="269"/>
+      <c r="U39" s="273"/>
       <c r="V39" s="126"/>
       <c r="W39" s="126"/>
     </row>
-    <row r="40" spans="1:23" s="127" customFormat="1" ht="45">
+    <row r="40" spans="1:23" s="127" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="116">
         <v>16</v>
       </c>
@@ -5276,13 +5326,13 @@
         <v>0</v>
       </c>
       <c r="T40" s="133"/>
-      <c r="U40" s="267" t="s">
+      <c r="U40" s="271" t="s">
         <v>91</v>
       </c>
       <c r="V40" s="135"/>
       <c r="W40" s="135"/>
     </row>
-    <row r="41" spans="1:23" s="127" customFormat="1" ht="45.75" customHeight="1">
+    <row r="41" spans="1:23" s="127" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="116">
         <v>17</v>
       </c>
@@ -5332,13 +5382,13 @@
       <c r="T41" s="133">
         <v>100</v>
       </c>
-      <c r="U41" s="268"/>
+      <c r="U41" s="272"/>
       <c r="V41" s="160" t="s">
         <v>92</v>
       </c>
       <c r="W41" s="160"/>
     </row>
-    <row r="42" spans="1:23" s="127" customFormat="1" ht="45.75" customHeight="1">
+    <row r="42" spans="1:23" s="127" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="116">
         <v>18</v>
       </c>
@@ -5372,11 +5422,11 @@
         <v>0</v>
       </c>
       <c r="T42" s="133"/>
-      <c r="U42" s="269"/>
+      <c r="U42" s="273"/>
       <c r="V42" s="126"/>
       <c r="W42" s="126"/>
     </row>
-    <row r="43" spans="1:23" s="127" customFormat="1">
+    <row r="43" spans="1:23" s="127" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="116"/>
       <c r="B43" s="227"/>
       <c r="C43" s="213"/>
@@ -5401,7 +5451,7 @@
       <c r="V43" s="126"/>
       <c r="W43" s="126"/>
     </row>
-    <row r="44" spans="1:23" s="127" customFormat="1" ht="30" customHeight="1">
+    <row r="44" spans="1:23" s="127" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="116"/>
       <c r="B44" s="231" t="s">
         <v>93</v>
@@ -5442,7 +5492,7 @@
       <c r="V44" s="126"/>
       <c r="W44" s="126"/>
     </row>
-    <row r="45" spans="1:23" s="127" customFormat="1" ht="49.5" customHeight="1">
+    <row r="45" spans="1:23" s="127" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="116">
         <v>19</v>
       </c>
@@ -5476,13 +5526,13 @@
         <v>0</v>
       </c>
       <c r="T45" s="133"/>
-      <c r="U45" s="267" t="s">
+      <c r="U45" s="271" t="s">
         <v>96</v>
       </c>
       <c r="V45" s="126"/>
       <c r="W45" s="126"/>
     </row>
-    <row r="46" spans="1:23" s="127" customFormat="1" ht="42.75" customHeight="1">
+    <row r="46" spans="1:23" s="127" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="116">
         <v>20</v>
       </c>
@@ -5516,11 +5566,11 @@
         <v>0</v>
       </c>
       <c r="T46" s="133"/>
-      <c r="U46" s="268"/>
+      <c r="U46" s="272"/>
       <c r="V46" s="135"/>
       <c r="W46" s="135"/>
     </row>
-    <row r="47" spans="1:23" s="127" customFormat="1" ht="42.75" customHeight="1">
+    <row r="47" spans="1:23" s="127" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="116">
         <v>21</v>
       </c>
@@ -5554,11 +5604,11 @@
         <v>0</v>
       </c>
       <c r="T47" s="133"/>
-      <c r="U47" s="269"/>
+      <c r="U47" s="273"/>
       <c r="V47" s="126"/>
       <c r="W47" s="126"/>
     </row>
-    <row r="48" spans="1:23" s="127" customFormat="1">
+    <row r="48" spans="1:23" s="127" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="116"/>
       <c r="B48" s="227"/>
       <c r="C48" s="213"/>
@@ -5583,7 +5633,7 @@
       <c r="V48" s="126"/>
       <c r="W48" s="126"/>
     </row>
-    <row r="49" spans="1:23" s="154" customFormat="1" ht="33" customHeight="1">
+    <row r="49" spans="1:23" s="154" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="144"/>
       <c r="B49" s="230" t="s">
         <v>97</v>
@@ -5626,7 +5676,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="50" spans="1:23" s="127" customFormat="1" ht="37.5" customHeight="1">
+    <row r="50" spans="1:23" s="127" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="116"/>
       <c r="B50" s="231" t="s">
         <v>99</v>
@@ -5667,7 +5717,7 @@
       <c r="V50" s="135"/>
       <c r="W50" s="135"/>
     </row>
-    <row r="51" spans="1:23" s="127" customFormat="1" ht="51" customHeight="1">
+    <row r="51" spans="1:23" s="127" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="116">
         <v>22</v>
       </c>
@@ -5701,13 +5751,13 @@
         <v>0</v>
       </c>
       <c r="T51" s="133"/>
-      <c r="U51" s="267" t="s">
+      <c r="U51" s="271" t="s">
         <v>102</v>
       </c>
       <c r="V51" s="167"/>
       <c r="W51" s="167"/>
     </row>
-    <row r="52" spans="1:23" s="127" customFormat="1" ht="45.75" customHeight="1">
+    <row r="52" spans="1:23" s="127" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="116">
         <v>23</v>
       </c>
@@ -5741,11 +5791,11 @@
         <v>0</v>
       </c>
       <c r="T52" s="133"/>
-      <c r="U52" s="268"/>
+      <c r="U52" s="272"/>
       <c r="V52" s="135"/>
       <c r="W52" s="135"/>
     </row>
-    <row r="53" spans="1:23" s="127" customFormat="1" ht="45.75" customHeight="1">
+    <row r="53" spans="1:23" s="127" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="116">
         <v>24</v>
       </c>
@@ -5779,11 +5829,11 @@
         <v>0</v>
       </c>
       <c r="T53" s="133"/>
-      <c r="U53" s="269"/>
+      <c r="U53" s="273"/>
       <c r="V53" s="135"/>
       <c r="W53" s="135"/>
     </row>
-    <row r="54" spans="1:23" s="127" customFormat="1" ht="65.25" customHeight="1">
+    <row r="54" spans="1:23" s="127" customFormat="1" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="116">
         <v>25</v>
       </c>
@@ -5817,13 +5867,13 @@
         <v>0</v>
       </c>
       <c r="T54" s="133"/>
-      <c r="U54" s="267" t="s">
+      <c r="U54" s="271" t="s">
         <v>104</v>
       </c>
       <c r="V54" s="135"/>
       <c r="W54" s="135"/>
     </row>
-    <row r="55" spans="1:23" s="127" customFormat="1" ht="43.5" customHeight="1">
+    <row r="55" spans="1:23" s="127" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="116">
         <v>26</v>
       </c>
@@ -5857,11 +5907,11 @@
         <v>0</v>
       </c>
       <c r="T55" s="133"/>
-      <c r="U55" s="268"/>
+      <c r="U55" s="272"/>
       <c r="V55" s="126"/>
       <c r="W55" s="126"/>
     </row>
-    <row r="56" spans="1:23" s="127" customFormat="1" ht="43.5" customHeight="1">
+    <row r="56" spans="1:23" s="127" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="116">
         <v>27</v>
       </c>
@@ -5895,11 +5945,11 @@
         <v>0</v>
       </c>
       <c r="T56" s="133"/>
-      <c r="U56" s="269"/>
+      <c r="U56" s="273"/>
       <c r="V56" s="135"/>
       <c r="W56" s="135"/>
     </row>
-    <row r="57" spans="1:23" s="127" customFormat="1">
+    <row r="57" spans="1:23" s="127" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="116"/>
       <c r="B57" s="227"/>
       <c r="C57" s="213"/>
@@ -5924,7 +5974,7 @@
       <c r="V57" s="126"/>
       <c r="W57" s="126"/>
     </row>
-    <row r="58" spans="1:23" s="154" customFormat="1" ht="47.25" customHeight="1">
+    <row r="58" spans="1:23" s="154" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="144"/>
       <c r="B58" s="230" t="s">
         <v>105</v>
@@ -5967,7 +6017,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="59" spans="1:23" s="127" customFormat="1" ht="24" customHeight="1">
+    <row r="59" spans="1:23" s="127" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="116"/>
       <c r="B59" s="231" t="s">
         <v>107</v>
@@ -6008,7 +6058,7 @@
       <c r="V59" s="160"/>
       <c r="W59" s="160"/>
     </row>
-    <row r="60" spans="1:23" s="127" customFormat="1" ht="183.75" customHeight="1">
+    <row r="60" spans="1:23" s="127" customFormat="1" ht="183.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="116">
         <v>28</v>
       </c>
@@ -6042,13 +6092,13 @@
         <v>0</v>
       </c>
       <c r="T60" s="133"/>
-      <c r="U60" s="277" t="s">
+      <c r="U60" s="274" t="s">
         <v>110</v>
       </c>
       <c r="V60" s="135"/>
       <c r="W60" s="135"/>
     </row>
-    <row r="61" spans="1:23" s="127" customFormat="1" ht="44.25" customHeight="1">
+    <row r="61" spans="1:23" s="127" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="116">
         <v>29</v>
       </c>
@@ -6092,11 +6142,11 @@
       <c r="T61" s="133">
         <v>100</v>
       </c>
-      <c r="U61" s="278"/>
+      <c r="U61" s="275"/>
       <c r="V61" s="135"/>
       <c r="W61" s="135"/>
     </row>
-    <row r="62" spans="1:23" s="127" customFormat="1" ht="44.25" customHeight="1">
+    <row r="62" spans="1:23" s="127" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="116">
         <v>30</v>
       </c>
@@ -6130,11 +6180,11 @@
         <v>0</v>
       </c>
       <c r="T62" s="133"/>
-      <c r="U62" s="279"/>
+      <c r="U62" s="276"/>
       <c r="V62" s="135"/>
       <c r="W62" s="135"/>
     </row>
-    <row r="63" spans="1:23" s="127" customFormat="1">
+    <row r="63" spans="1:23" s="127" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="116"/>
       <c r="B63" s="227"/>
       <c r="C63" s="213"/>
@@ -6159,7 +6209,7 @@
       <c r="V63" s="126"/>
       <c r="W63" s="126"/>
     </row>
-    <row r="64" spans="1:23" s="154" customFormat="1" ht="47.25" customHeight="1">
+    <row r="64" spans="1:23" s="154" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="144"/>
       <c r="B64" s="230" t="s">
         <v>113</v>
@@ -6202,7 +6252,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="65" spans="1:23" s="127" customFormat="1" ht="55.5" customHeight="1">
+    <row r="65" spans="1:23" s="127" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="116"/>
       <c r="B65" s="231" t="s">
         <v>115</v>
@@ -6243,7 +6293,7 @@
       <c r="V65" s="135"/>
       <c r="W65" s="135"/>
     </row>
-    <row r="66" spans="1:23" s="127" customFormat="1" ht="78.75" customHeight="1">
+    <row r="66" spans="1:23" s="127" customFormat="1" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="116">
         <v>31</v>
       </c>
@@ -6277,13 +6327,13 @@
         <v>0</v>
       </c>
       <c r="T66" s="133"/>
-      <c r="U66" s="267" t="s">
+      <c r="U66" s="271" t="s">
         <v>118</v>
       </c>
       <c r="V66" s="135"/>
       <c r="W66" s="135"/>
     </row>
-    <row r="67" spans="1:23" s="127" customFormat="1" ht="46.5" customHeight="1">
+    <row r="67" spans="1:23" s="127" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="116">
         <v>32</v>
       </c>
@@ -6317,11 +6367,11 @@
         <v>0</v>
       </c>
       <c r="T67" s="133"/>
-      <c r="U67" s="268"/>
+      <c r="U67" s="272"/>
       <c r="V67" s="135"/>
       <c r="W67" s="135"/>
     </row>
-    <row r="68" spans="1:23" s="127" customFormat="1" ht="46.5" customHeight="1">
+    <row r="68" spans="1:23" s="127" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="116">
         <v>33</v>
       </c>
@@ -6355,11 +6405,11 @@
         <v>0</v>
       </c>
       <c r="T68" s="133"/>
-      <c r="U68" s="269"/>
+      <c r="U68" s="273"/>
       <c r="V68" s="135"/>
       <c r="W68" s="135"/>
     </row>
-    <row r="69" spans="1:23" s="127" customFormat="1" ht="63" customHeight="1">
+    <row r="69" spans="1:23" s="127" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="116">
         <v>34</v>
       </c>
@@ -6393,13 +6443,13 @@
         <v>0</v>
       </c>
       <c r="T69" s="133"/>
-      <c r="U69" s="267" t="s">
+      <c r="U69" s="271" t="s">
         <v>120</v>
       </c>
       <c r="V69" s="135"/>
       <c r="W69" s="135"/>
     </row>
-    <row r="70" spans="1:23" s="127" customFormat="1" ht="45" customHeight="1">
+    <row r="70" spans="1:23" s="127" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="116">
         <v>35</v>
       </c>
@@ -6433,11 +6483,11 @@
         <v>0</v>
       </c>
       <c r="T70" s="133"/>
-      <c r="U70" s="268"/>
+      <c r="U70" s="272"/>
       <c r="V70" s="135"/>
       <c r="W70" s="135"/>
     </row>
-    <row r="71" spans="1:23" s="127" customFormat="1" ht="45" customHeight="1">
+    <row r="71" spans="1:23" s="127" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="116">
         <v>36</v>
       </c>
@@ -6471,11 +6521,11 @@
         <v>0</v>
       </c>
       <c r="T71" s="133"/>
-      <c r="U71" s="269"/>
+      <c r="U71" s="273"/>
       <c r="V71" s="135"/>
       <c r="W71" s="135"/>
     </row>
-    <row r="72" spans="1:23" s="127" customFormat="1" ht="68.25" customHeight="1">
+    <row r="72" spans="1:23" s="127" customFormat="1" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="116">
         <v>37</v>
       </c>
@@ -6509,13 +6559,13 @@
         <v>0</v>
       </c>
       <c r="T72" s="133"/>
-      <c r="U72" s="267" t="s">
+      <c r="U72" s="271" t="s">
         <v>122</v>
       </c>
       <c r="V72" s="135"/>
       <c r="W72" s="135"/>
     </row>
-    <row r="73" spans="1:23" s="127" customFormat="1" ht="42.75" customHeight="1">
+    <row r="73" spans="1:23" s="127" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="116">
         <v>38</v>
       </c>
@@ -6549,11 +6599,11 @@
         <v>0</v>
       </c>
       <c r="T73" s="133"/>
-      <c r="U73" s="268"/>
+      <c r="U73" s="272"/>
       <c r="V73" s="135"/>
       <c r="W73" s="135"/>
     </row>
-    <row r="74" spans="1:23" s="127" customFormat="1" ht="42.75" customHeight="1">
+    <row r="74" spans="1:23" s="127" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="116">
         <v>39</v>
       </c>
@@ -6587,11 +6637,11 @@
         <v>0</v>
       </c>
       <c r="T74" s="133"/>
-      <c r="U74" s="269"/>
+      <c r="U74" s="273"/>
       <c r="V74" s="135"/>
       <c r="W74" s="135"/>
     </row>
-    <row r="75" spans="1:23" s="127" customFormat="1">
+    <row r="75" spans="1:23" s="127" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="116"/>
       <c r="B75" s="227"/>
       <c r="C75" s="218"/>
@@ -6616,7 +6666,7 @@
       <c r="V75" s="126"/>
       <c r="W75" s="126"/>
     </row>
-    <row r="76" spans="1:23" s="127" customFormat="1" ht="67.5" customHeight="1">
+    <row r="76" spans="1:23" s="127" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="116"/>
       <c r="B76" s="231" t="s">
         <v>123</v>
@@ -6657,7 +6707,7 @@
       <c r="V76" s="135"/>
       <c r="W76" s="135"/>
     </row>
-    <row r="77" spans="1:23" s="127" customFormat="1" ht="52.5" customHeight="1">
+    <row r="77" spans="1:23" s="127" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="116">
         <v>40</v>
       </c>
@@ -6693,13 +6743,13 @@
         <v>0</v>
       </c>
       <c r="T77" s="133"/>
-      <c r="U77" s="267" t="s">
+      <c r="U77" s="271" t="s">
         <v>127</v>
       </c>
       <c r="V77" s="135"/>
       <c r="W77" s="135"/>
     </row>
-    <row r="78" spans="1:23" s="127" customFormat="1" ht="42.75" customHeight="1">
+    <row r="78" spans="1:23" s="127" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="116">
         <v>41</v>
       </c>
@@ -6733,11 +6783,11 @@
         <v>0</v>
       </c>
       <c r="T78" s="133"/>
-      <c r="U78" s="268"/>
+      <c r="U78" s="272"/>
       <c r="V78" s="135"/>
       <c r="W78" s="135"/>
     </row>
-    <row r="79" spans="1:23" s="127" customFormat="1" ht="42.75" customHeight="1">
+    <row r="79" spans="1:23" s="127" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="116">
         <v>42</v>
       </c>
@@ -6771,11 +6821,11 @@
         <v>0</v>
       </c>
       <c r="T79" s="133"/>
-      <c r="U79" s="269"/>
+      <c r="U79" s="273"/>
       <c r="V79" s="135"/>
       <c r="W79" s="135"/>
     </row>
-    <row r="80" spans="1:23" s="127" customFormat="1" ht="65.25" customHeight="1">
+    <row r="80" spans="1:23" s="127" customFormat="1" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="116">
         <v>43</v>
       </c>
@@ -6809,13 +6859,13 @@
         <v>0</v>
       </c>
       <c r="T80" s="133"/>
-      <c r="U80" s="267" t="s">
+      <c r="U80" s="271" t="s">
         <v>129</v>
       </c>
       <c r="V80" s="135"/>
       <c r="W80" s="135"/>
     </row>
-    <row r="81" spans="1:23" s="127" customFormat="1" ht="36" customHeight="1">
+    <row r="81" spans="1:23" s="127" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="116">
         <v>44</v>
       </c>
@@ -6849,11 +6899,11 @@
         <v>0</v>
       </c>
       <c r="T81" s="133"/>
-      <c r="U81" s="268"/>
+      <c r="U81" s="272"/>
       <c r="V81" s="135"/>
       <c r="W81" s="135"/>
     </row>
-    <row r="82" spans="1:23" s="127" customFormat="1" ht="36" customHeight="1">
+    <row r="82" spans="1:23" s="127" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="116">
         <v>45</v>
       </c>
@@ -6887,11 +6937,11 @@
         <v>0</v>
       </c>
       <c r="T82" s="133"/>
-      <c r="U82" s="269"/>
+      <c r="U82" s="273"/>
       <c r="V82" s="126"/>
       <c r="W82" s="126"/>
     </row>
-    <row r="83" spans="1:23" s="127" customFormat="1">
+    <row r="83" spans="1:23" s="127" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="116"/>
       <c r="B83" s="227"/>
       <c r="C83" s="218"/>
@@ -6916,7 +6966,7 @@
       <c r="V83" s="126"/>
       <c r="W83" s="126"/>
     </row>
-    <row r="84" spans="1:23" s="154" customFormat="1" ht="102" customHeight="1">
+    <row r="84" spans="1:23" s="154" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="144"/>
       <c r="B84" s="230" t="s">
         <v>130</v>
@@ -6959,7 +7009,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="85" spans="1:23" s="127" customFormat="1" ht="54.75" customHeight="1">
+    <row r="85" spans="1:23" s="127" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="116"/>
       <c r="B85" s="231" t="s">
         <v>132</v>
@@ -7000,7 +7050,7 @@
       <c r="V85" s="126"/>
       <c r="W85" s="126"/>
     </row>
-    <row r="86" spans="1:23" s="127" customFormat="1" ht="46.5" customHeight="1">
+    <row r="86" spans="1:23" s="127" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="116">
         <v>46</v>
       </c>
@@ -7034,13 +7084,13 @@
         <v>0</v>
       </c>
       <c r="T86" s="133"/>
-      <c r="U86" s="274" t="s">
+      <c r="U86" s="277" t="s">
         <v>135</v>
       </c>
       <c r="V86" s="135"/>
       <c r="W86" s="135"/>
     </row>
-    <row r="87" spans="1:23" s="143" customFormat="1" ht="60.75" customHeight="1">
+    <row r="87" spans="1:23" s="143" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="116">
         <v>47</v>
       </c>
@@ -7057,9 +7107,9 @@
       <c r="F87" s="139"/>
       <c r="G87" s="122"/>
       <c r="H87" s="122"/>
-      <c r="I87" s="280"/>
-      <c r="J87" s="281"/>
-      <c r="K87" s="282"/>
+      <c r="I87" s="268"/>
+      <c r="J87" s="269"/>
+      <c r="K87" s="270"/>
       <c r="L87" s="71"/>
       <c r="M87" s="71"/>
       <c r="N87" s="132" t="s">
@@ -7074,11 +7124,11 @@
         <v>0</v>
       </c>
       <c r="T87" s="133"/>
-      <c r="U87" s="275"/>
+      <c r="U87" s="278"/>
       <c r="V87" s="160"/>
       <c r="W87" s="160"/>
     </row>
-    <row r="88" spans="1:23" s="143" customFormat="1" ht="54.75" customHeight="1">
+    <row r="88" spans="1:23" s="143" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="116">
         <v>48</v>
       </c>
@@ -7095,9 +7145,9 @@
       <c r="F88" s="139"/>
       <c r="G88" s="122"/>
       <c r="H88" s="122"/>
-      <c r="I88" s="280"/>
-      <c r="J88" s="281"/>
-      <c r="K88" s="282"/>
+      <c r="I88" s="268"/>
+      <c r="J88" s="269"/>
+      <c r="K88" s="270"/>
       <c r="L88" s="71"/>
       <c r="M88" s="71"/>
       <c r="N88" s="132" t="s">
@@ -7112,11 +7162,11 @@
         <v>0</v>
       </c>
       <c r="T88" s="133"/>
-      <c r="U88" s="275"/>
+      <c r="U88" s="278"/>
       <c r="V88" s="160"/>
       <c r="W88" s="160"/>
     </row>
-    <row r="89" spans="1:23" s="143" customFormat="1" ht="50.25" customHeight="1">
+    <row r="89" spans="1:23" s="143" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="116">
         <v>49</v>
       </c>
@@ -7150,11 +7200,11 @@
         <v>0</v>
       </c>
       <c r="T89" s="133"/>
-      <c r="U89" s="275"/>
+      <c r="U89" s="278"/>
       <c r="V89" s="173"/>
       <c r="W89" s="173"/>
     </row>
-    <row r="90" spans="1:23" s="143" customFormat="1" ht="51.75" customHeight="1">
+    <row r="90" spans="1:23" s="143" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="116">
         <v>50</v>
       </c>
@@ -7188,11 +7238,11 @@
         <v>0</v>
       </c>
       <c r="T90" s="133"/>
-      <c r="U90" s="275"/>
+      <c r="U90" s="278"/>
       <c r="V90" s="174"/>
       <c r="W90" s="174"/>
     </row>
-    <row r="91" spans="1:23" s="143" customFormat="1" ht="69" customHeight="1">
+    <row r="91" spans="1:23" s="143" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="116">
         <v>51</v>
       </c>
@@ -7226,11 +7276,11 @@
         <v>0</v>
       </c>
       <c r="T91" s="133"/>
-      <c r="U91" s="276"/>
+      <c r="U91" s="279"/>
       <c r="V91" s="174"/>
       <c r="W91" s="174"/>
     </row>
-    <row r="92" spans="1:23" s="127" customFormat="1">
+    <row r="92" spans="1:23" s="127" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="116"/>
       <c r="B92" s="227"/>
       <c r="C92" s="213"/>
@@ -7255,7 +7305,7 @@
       <c r="V92" s="132"/>
       <c r="W92" s="132"/>
     </row>
-    <row r="93" spans="1:23" s="127" customFormat="1" ht="75" customHeight="1">
+    <row r="93" spans="1:23" s="127" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="116"/>
       <c r="B93" s="231" t="s">
         <v>141</v>
@@ -7296,7 +7346,7 @@
       <c r="V93" s="135"/>
       <c r="W93" s="135"/>
     </row>
-    <row r="94" spans="1:23" s="127" customFormat="1" ht="99.75" customHeight="1">
+    <row r="94" spans="1:23" s="127" customFormat="1" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="116">
         <v>52</v>
       </c>
@@ -7330,13 +7380,13 @@
         <v>0</v>
       </c>
       <c r="T94" s="133"/>
-      <c r="U94" s="277" t="s">
+      <c r="U94" s="274" t="s">
         <v>144</v>
       </c>
       <c r="V94" s="135"/>
       <c r="W94" s="135"/>
     </row>
-    <row r="95" spans="1:23" s="127" customFormat="1" ht="69" customHeight="1">
+    <row r="95" spans="1:23" s="127" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="116">
         <v>53</v>
       </c>
@@ -7380,11 +7430,11 @@
       <c r="T95" s="133">
         <v>100</v>
       </c>
-      <c r="U95" s="278"/>
+      <c r="U95" s="275"/>
       <c r="V95" s="135"/>
       <c r="W95" s="135"/>
     </row>
-    <row r="96" spans="1:23" s="127" customFormat="1" ht="55.5" customHeight="1">
+    <row r="96" spans="1:23" s="127" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="116">
         <v>54</v>
       </c>
@@ -7418,11 +7468,11 @@
         <v>0</v>
       </c>
       <c r="T96" s="133"/>
-      <c r="U96" s="279"/>
+      <c r="U96" s="276"/>
       <c r="V96" s="135"/>
       <c r="W96" s="135"/>
     </row>
-    <row r="97" spans="1:23" s="127" customFormat="1" ht="101.25" customHeight="1">
+    <row r="97" spans="1:23" s="127" customFormat="1" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="116">
         <v>55</v>
       </c>
@@ -7456,13 +7506,13 @@
         <v>0</v>
       </c>
       <c r="T97" s="133"/>
-      <c r="U97" s="277" t="s">
+      <c r="U97" s="274" t="s">
         <v>148</v>
       </c>
       <c r="V97" s="135"/>
       <c r="W97" s="135"/>
     </row>
-    <row r="98" spans="1:23" s="127" customFormat="1" ht="61.5" customHeight="1">
+    <row r="98" spans="1:23" s="127" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="116">
         <v>56</v>
       </c>
@@ -7506,11 +7556,11 @@
       <c r="T98" s="133">
         <v>100</v>
       </c>
-      <c r="U98" s="278"/>
+      <c r="U98" s="275"/>
       <c r="V98" s="135"/>
       <c r="W98" s="135"/>
     </row>
-    <row r="99" spans="1:23" s="127" customFormat="1" ht="43.5" customHeight="1">
+    <row r="99" spans="1:23" s="127" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="116">
         <v>57</v>
       </c>
@@ -7544,11 +7594,11 @@
         <v>0</v>
       </c>
       <c r="T99" s="133"/>
-      <c r="U99" s="279"/>
+      <c r="U99" s="276"/>
       <c r="V99" s="135"/>
       <c r="W99" s="135"/>
     </row>
-    <row r="100" spans="1:23" s="127" customFormat="1" ht="122.25" customHeight="1">
+    <row r="100" spans="1:23" s="127" customFormat="1" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="116">
         <v>58</v>
       </c>
@@ -7582,13 +7632,13 @@
         <v>0</v>
       </c>
       <c r="T100" s="133"/>
-      <c r="U100" s="277" t="s">
+      <c r="U100" s="274" t="s">
         <v>150</v>
       </c>
       <c r="V100" s="135"/>
       <c r="W100" s="135"/>
     </row>
-    <row r="101" spans="1:23" s="127" customFormat="1" ht="45.75" customHeight="1">
+    <row r="101" spans="1:23" s="127" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="116">
         <v>59</v>
       </c>
@@ -7622,11 +7672,11 @@
         <v>0</v>
       </c>
       <c r="T101" s="133"/>
-      <c r="U101" s="278"/>
+      <c r="U101" s="275"/>
       <c r="V101" s="135"/>
       <c r="W101" s="135"/>
     </row>
-    <row r="102" spans="1:23" s="127" customFormat="1" ht="37.5" customHeight="1">
+    <row r="102" spans="1:23" s="127" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="116">
         <v>60</v>
       </c>
@@ -7660,11 +7710,11 @@
         <v>0</v>
       </c>
       <c r="T102" s="133"/>
-      <c r="U102" s="279"/>
+      <c r="U102" s="276"/>
       <c r="V102" s="135"/>
       <c r="W102" s="135"/>
     </row>
-    <row r="103" spans="1:23" s="127" customFormat="1">
+    <row r="103" spans="1:23" s="127" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="116"/>
       <c r="B103" s="227"/>
       <c r="C103" s="213"/>
@@ -7689,7 +7739,7 @@
       <c r="V103" s="126"/>
       <c r="W103" s="126"/>
     </row>
-    <row r="104" spans="1:23" s="127" customFormat="1" ht="61.5" customHeight="1">
+    <row r="104" spans="1:23" s="127" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="116"/>
       <c r="B104" s="231" t="s">
         <v>151</v>
@@ -7730,7 +7780,7 @@
       <c r="V104" s="135"/>
       <c r="W104" s="135"/>
     </row>
-    <row r="105" spans="1:23" s="127" customFormat="1" ht="45">
+    <row r="105" spans="1:23" s="127" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A105" s="116">
         <v>61</v>
       </c>
@@ -7770,7 +7820,7 @@
       <c r="V105" s="135"/>
       <c r="W105" s="135"/>
     </row>
-    <row r="106" spans="1:23" s="127" customFormat="1" ht="75.75" customHeight="1">
+    <row r="106" spans="1:23" s="127" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="116">
         <v>62</v>
       </c>
@@ -7810,7 +7860,7 @@
       <c r="V106" s="135"/>
       <c r="W106" s="135"/>
     </row>
-    <row r="107" spans="1:23" s="127" customFormat="1" ht="75" customHeight="1">
+    <row r="107" spans="1:23" s="127" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="116">
         <v>63</v>
       </c>
@@ -7850,7 +7900,7 @@
       <c r="V107" s="135"/>
       <c r="W107" s="135"/>
     </row>
-    <row r="108" spans="1:23" s="127" customFormat="1">
+    <row r="108" spans="1:23" s="127" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="116"/>
       <c r="B108" s="227"/>
       <c r="C108" s="213"/>
@@ -7875,7 +7925,7 @@
       <c r="V108" s="126"/>
       <c r="W108" s="126"/>
     </row>
-    <row r="109" spans="1:23" s="154" customFormat="1" ht="47.25" customHeight="1">
+    <row r="109" spans="1:23" s="154" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="144"/>
       <c r="B109" s="228" t="s">
         <v>159</v>
@@ -7918,7 +7968,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="110" spans="1:23" s="127" customFormat="1" ht="37.5" customHeight="1">
+    <row r="110" spans="1:23" s="127" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="116"/>
       <c r="B110" s="227" t="s">
         <v>161</v>
@@ -7959,7 +8009,7 @@
       <c r="V110" s="135"/>
       <c r="W110" s="135"/>
     </row>
-    <row r="111" spans="1:23" s="127" customFormat="1" ht="39.75" customHeight="1">
+    <row r="111" spans="1:23" s="127" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="116">
         <v>64</v>
       </c>
@@ -7993,13 +8043,13 @@
         <v>0</v>
       </c>
       <c r="T111" s="133"/>
-      <c r="U111" s="277" t="s">
+      <c r="U111" s="274" t="s">
         <v>158</v>
       </c>
       <c r="V111" s="135"/>
       <c r="W111" s="135"/>
     </row>
-    <row r="112" spans="1:23" s="127" customFormat="1" ht="39.75" customHeight="1">
+    <row r="112" spans="1:23" s="127" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="116">
         <v>65</v>
       </c>
@@ -8038,13 +8088,13 @@
       <c r="R112" s="132"/>
       <c r="S112" s="123"/>
       <c r="T112" s="133"/>
-      <c r="U112" s="278"/>
+      <c r="U112" s="275"/>
       <c r="V112" s="135" t="s">
         <v>166</v>
       </c>
       <c r="W112" s="135"/>
     </row>
-    <row r="113" spans="1:23" s="143" customFormat="1" ht="47.25" customHeight="1">
+    <row r="113" spans="1:23" s="143" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="116">
         <v>66</v>
       </c>
@@ -8078,11 +8128,11 @@
         <v>0</v>
       </c>
       <c r="T113" s="133"/>
-      <c r="U113" s="279"/>
+      <c r="U113" s="276"/>
       <c r="V113" s="135"/>
       <c r="W113" s="135"/>
     </row>
-    <row r="114" spans="1:23" s="127" customFormat="1" ht="69.75" customHeight="1">
+    <row r="114" spans="1:23" s="127" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="116">
         <v>67</v>
       </c>
@@ -8116,13 +8166,13 @@
         <v>0</v>
       </c>
       <c r="T114" s="133"/>
-      <c r="U114" s="267" t="s">
+      <c r="U114" s="271" t="s">
         <v>168</v>
       </c>
       <c r="V114" s="126"/>
       <c r="W114" s="126"/>
     </row>
-    <row r="115" spans="1:23" s="127" customFormat="1" ht="40.5" customHeight="1">
+    <row r="115" spans="1:23" s="127" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="116">
         <v>68</v>
       </c>
@@ -8164,11 +8214,11 @@
         <v>0</v>
       </c>
       <c r="T115" s="133"/>
-      <c r="U115" s="268"/>
+      <c r="U115" s="272"/>
       <c r="V115" s="135"/>
       <c r="W115" s="135"/>
     </row>
-    <row r="116" spans="1:23" s="127" customFormat="1" ht="40.5" customHeight="1">
+    <row r="116" spans="1:23" s="127" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="116">
         <v>69</v>
       </c>
@@ -8202,11 +8252,11 @@
         <v>0</v>
       </c>
       <c r="T116" s="133"/>
-      <c r="U116" s="269"/>
+      <c r="U116" s="273"/>
       <c r="V116" s="135"/>
       <c r="W116" s="135"/>
     </row>
-    <row r="117" spans="1:23" s="127" customFormat="1" ht="45.75" customHeight="1">
+    <row r="117" spans="1:23" s="127" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="116">
         <v>70</v>
       </c>
@@ -8240,13 +8290,13 @@
         <v>0</v>
       </c>
       <c r="T117" s="133"/>
-      <c r="U117" s="267" t="s">
+      <c r="U117" s="271" t="s">
         <v>172</v>
       </c>
       <c r="V117" s="135"/>
       <c r="W117" s="135"/>
     </row>
-    <row r="118" spans="1:23" s="127" customFormat="1" ht="45.75" customHeight="1">
+    <row r="118" spans="1:23" s="127" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="116">
         <v>71</v>
       </c>
@@ -8288,11 +8338,11 @@
         <v>0</v>
       </c>
       <c r="T118" s="133"/>
-      <c r="U118" s="268"/>
+      <c r="U118" s="272"/>
       <c r="V118" s="135"/>
       <c r="W118" s="135"/>
     </row>
-    <row r="119" spans="1:23" s="127" customFormat="1" ht="45.75" customHeight="1">
+    <row r="119" spans="1:23" s="127" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="116">
         <v>72</v>
       </c>
@@ -8326,11 +8376,11 @@
         <v>0</v>
       </c>
       <c r="T119" s="133"/>
-      <c r="U119" s="269"/>
+      <c r="U119" s="273"/>
       <c r="V119" s="135"/>
       <c r="W119" s="135"/>
     </row>
-    <row r="120" spans="1:23" s="127" customFormat="1" ht="60" customHeight="1">
+    <row r="120" spans="1:23" s="127" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="116">
         <v>73</v>
       </c>
@@ -8364,13 +8414,13 @@
         <v>0</v>
       </c>
       <c r="T120" s="133"/>
-      <c r="U120" s="267" t="s">
+      <c r="U120" s="271" t="s">
         <v>174</v>
       </c>
       <c r="V120" s="135"/>
       <c r="W120" s="135"/>
     </row>
-    <row r="121" spans="1:23" s="127" customFormat="1" ht="45.75" customHeight="1">
+    <row r="121" spans="1:23" s="127" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="116">
         <v>74</v>
       </c>
@@ -8412,13 +8462,13 @@
         <v>0</v>
       </c>
       <c r="T121" s="133"/>
-      <c r="U121" s="268"/>
+      <c r="U121" s="272"/>
       <c r="V121" s="135" t="s">
         <v>166</v>
       </c>
       <c r="W121" s="135"/>
     </row>
-    <row r="122" spans="1:23" s="127" customFormat="1" ht="45.75" customHeight="1">
+    <row r="122" spans="1:23" s="127" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="116">
         <v>75</v>
       </c>
@@ -8452,11 +8502,11 @@
         <v>0</v>
       </c>
       <c r="T122" s="133"/>
-      <c r="U122" s="269"/>
+      <c r="U122" s="273"/>
       <c r="V122" s="135"/>
       <c r="W122" s="135"/>
     </row>
-    <row r="123" spans="1:23" s="127" customFormat="1" ht="50.25" customHeight="1">
+    <row r="123" spans="1:23" s="127" customFormat="1" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="116">
         <v>76</v>
       </c>
@@ -8490,13 +8540,13 @@
         <v>0</v>
       </c>
       <c r="T123" s="133"/>
-      <c r="U123" s="267" t="s">
+      <c r="U123" s="271" t="s">
         <v>178</v>
       </c>
       <c r="V123" s="126"/>
       <c r="W123" s="126"/>
     </row>
-    <row r="124" spans="1:23" s="127" customFormat="1" ht="41.25" customHeight="1">
+    <row r="124" spans="1:23" s="127" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="116">
         <v>77</v>
       </c>
@@ -8530,11 +8580,11 @@
         <v>0</v>
       </c>
       <c r="T124" s="133"/>
-      <c r="U124" s="268"/>
+      <c r="U124" s="272"/>
       <c r="V124" s="135"/>
       <c r="W124" s="135"/>
     </row>
-    <row r="125" spans="1:23" s="127" customFormat="1" ht="41.25" customHeight="1">
+    <row r="125" spans="1:23" s="127" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="116">
         <v>78</v>
       </c>
@@ -8568,11 +8618,11 @@
         <v>0</v>
       </c>
       <c r="T125" s="133"/>
-      <c r="U125" s="269"/>
+      <c r="U125" s="273"/>
       <c r="V125" s="135"/>
       <c r="W125" s="135"/>
     </row>
-    <row r="126" spans="1:23" s="127" customFormat="1" ht="46.5" customHeight="1">
+    <row r="126" spans="1:23" s="127" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="116">
         <v>79</v>
       </c>
@@ -8606,13 +8656,13 @@
         <v>0</v>
       </c>
       <c r="T126" s="133"/>
-      <c r="U126" s="267" t="s">
+      <c r="U126" s="271" t="s">
         <v>178</v>
       </c>
       <c r="V126" s="135"/>
       <c r="W126" s="135"/>
     </row>
-    <row r="127" spans="1:23" s="185" customFormat="1" ht="46.5" customHeight="1">
+    <row r="127" spans="1:23" s="185" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="116">
         <v>80</v>
       </c>
@@ -8646,11 +8696,11 @@
         <v>0</v>
       </c>
       <c r="T127" s="133"/>
-      <c r="U127" s="268"/>
+      <c r="U127" s="272"/>
       <c r="V127" s="160"/>
       <c r="W127" s="160"/>
     </row>
-    <row r="128" spans="1:23" s="185" customFormat="1" ht="46.5" customHeight="1">
+    <row r="128" spans="1:23" s="185" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="116">
         <v>81</v>
       </c>
@@ -8684,11 +8734,11 @@
         <v>0</v>
       </c>
       <c r="T128" s="133"/>
-      <c r="U128" s="269"/>
+      <c r="U128" s="273"/>
       <c r="V128" s="160"/>
       <c r="W128" s="160"/>
     </row>
-    <row r="129" spans="1:23" s="185" customFormat="1" ht="46.5" customHeight="1">
+    <row r="129" spans="1:23" s="185" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="116">
         <v>82</v>
       </c>
@@ -8722,13 +8772,13 @@
         <v>0</v>
       </c>
       <c r="T129" s="133"/>
-      <c r="U129" s="267" t="s">
+      <c r="U129" s="271" t="s">
         <v>181</v>
       </c>
       <c r="V129" s="160"/>
       <c r="W129" s="160"/>
     </row>
-    <row r="130" spans="1:23" s="185" customFormat="1" ht="46.5" customHeight="1">
+    <row r="130" spans="1:23" s="185" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="116">
         <v>83</v>
       </c>
@@ -8770,11 +8820,11 @@
         <v>0</v>
       </c>
       <c r="T130" s="133"/>
-      <c r="U130" s="268"/>
+      <c r="U130" s="272"/>
       <c r="V130" s="160"/>
       <c r="W130" s="160"/>
     </row>
-    <row r="131" spans="1:23" s="185" customFormat="1" ht="46.5" customHeight="1">
+    <row r="131" spans="1:23" s="185" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="116">
         <v>84</v>
       </c>
@@ -8808,11 +8858,11 @@
         <v>0</v>
       </c>
       <c r="T131" s="133"/>
-      <c r="U131" s="269"/>
+      <c r="U131" s="273"/>
       <c r="V131" s="160"/>
       <c r="W131" s="160"/>
     </row>
-    <row r="132" spans="1:23" s="185" customFormat="1" ht="46.5" customHeight="1">
+    <row r="132" spans="1:23" s="185" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="116">
         <v>85</v>
       </c>
@@ -8846,13 +8896,13 @@
         <v>0</v>
       </c>
       <c r="T132" s="133"/>
-      <c r="U132" s="267" t="s">
+      <c r="U132" s="271" t="s">
         <v>96</v>
       </c>
       <c r="V132" s="160"/>
       <c r="W132" s="160"/>
     </row>
-    <row r="133" spans="1:23" s="185" customFormat="1" ht="46.5" customHeight="1">
+    <row r="133" spans="1:23" s="185" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="116">
         <v>86</v>
       </c>
@@ -8902,13 +8952,13 @@
       <c r="T133" s="133">
         <v>100</v>
       </c>
-      <c r="U133" s="268"/>
+      <c r="U133" s="272"/>
       <c r="V133" s="160" t="s">
         <v>185</v>
       </c>
       <c r="W133" s="160"/>
     </row>
-    <row r="134" spans="1:23" s="185" customFormat="1" ht="46.5" customHeight="1">
+    <row r="134" spans="1:23" s="185" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="116">
         <v>87</v>
       </c>
@@ -8942,11 +8992,11 @@
         <v>0</v>
       </c>
       <c r="T134" s="133"/>
-      <c r="U134" s="269"/>
+      <c r="U134" s="273"/>
       <c r="V134" s="160"/>
       <c r="W134" s="160"/>
     </row>
-    <row r="135" spans="1:23" s="185" customFormat="1" ht="46.5" customHeight="1">
+    <row r="135" spans="1:23" s="185" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="116">
         <v>88</v>
       </c>
@@ -8980,13 +9030,13 @@
         <v>0</v>
       </c>
       <c r="T135" s="133"/>
-      <c r="U135" s="267" t="s">
+      <c r="U135" s="271" t="s">
         <v>96</v>
       </c>
       <c r="V135" s="160"/>
       <c r="W135" s="160"/>
     </row>
-    <row r="136" spans="1:23" s="185" customFormat="1" ht="46.5" customHeight="1">
+    <row r="136" spans="1:23" s="185" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="116">
         <v>89</v>
       </c>
@@ -9034,13 +9084,13 @@
       <c r="T136" s="133">
         <v>100</v>
       </c>
-      <c r="U136" s="268"/>
+      <c r="U136" s="272"/>
       <c r="V136" s="160" t="s">
         <v>189</v>
       </c>
       <c r="W136" s="160"/>
     </row>
-    <row r="137" spans="1:23" s="185" customFormat="1" ht="46.5" customHeight="1">
+    <row r="137" spans="1:23" s="185" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="116">
         <v>90</v>
       </c>
@@ -9074,11 +9124,11 @@
         <v>0</v>
       </c>
       <c r="T137" s="133"/>
-      <c r="U137" s="269"/>
+      <c r="U137" s="273"/>
       <c r="V137" s="160"/>
       <c r="W137" s="160"/>
     </row>
-    <row r="138" spans="1:23" s="185" customFormat="1">
+    <row r="138" spans="1:23" s="185" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="116"/>
       <c r="B138" s="227"/>
       <c r="C138" s="213"/>
@@ -9103,7 +9153,7 @@
       <c r="V138" s="187"/>
       <c r="W138" s="187"/>
     </row>
-    <row r="139" spans="1:23" s="154" customFormat="1" ht="34.5" customHeight="1">
+    <row r="139" spans="1:23" s="154" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="144"/>
       <c r="B139" s="228" t="s">
         <v>190</v>
@@ -9146,7 +9196,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="140" spans="1:23" s="127" customFormat="1" ht="34.5" customHeight="1">
+    <row r="140" spans="1:23" s="127" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="116"/>
       <c r="B140" s="227" t="s">
         <v>192</v>
@@ -9187,7 +9237,7 @@
       <c r="V140" s="126"/>
       <c r="W140" s="126"/>
     </row>
-    <row r="141" spans="1:23" s="185" customFormat="1" ht="58.5" customHeight="1">
+    <row r="141" spans="1:23" s="185" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="116">
         <v>91</v>
       </c>
@@ -9227,7 +9277,7 @@
       <c r="V141" s="187"/>
       <c r="W141" s="187"/>
     </row>
-    <row r="142" spans="1:23" s="185" customFormat="1">
+    <row r="142" spans="1:23" s="185" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A142" s="116"/>
       <c r="B142" s="227"/>
       <c r="C142" s="213"/>
@@ -9252,7 +9302,7 @@
       <c r="V142" s="187"/>
       <c r="W142" s="187"/>
     </row>
-    <row r="143" spans="1:23" s="154" customFormat="1" ht="63" customHeight="1">
+    <row r="143" spans="1:23" s="154" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="144"/>
       <c r="B143" s="228" t="s">
         <v>195</v>
@@ -9295,7 +9345,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="144" spans="1:23" s="127" customFormat="1" ht="48" customHeight="1">
+    <row r="144" spans="1:23" s="127" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="116"/>
       <c r="B144" s="227" t="s">
         <v>197</v>
@@ -9336,7 +9386,7 @@
       <c r="V144" s="126"/>
       <c r="W144" s="126"/>
     </row>
-    <row r="145" spans="1:23" s="185" customFormat="1" ht="69" customHeight="1">
+    <row r="145" spans="1:23" s="185" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="116">
         <v>92</v>
       </c>
@@ -9376,7 +9426,7 @@
       <c r="V145" s="160"/>
       <c r="W145" s="160"/>
     </row>
-    <row r="146" spans="1:23" s="185" customFormat="1" ht="48" customHeight="1">
+    <row r="146" spans="1:23" s="185" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="116">
         <v>93</v>
       </c>
@@ -9416,7 +9466,7 @@
       <c r="V146" s="160"/>
       <c r="W146" s="160"/>
     </row>
-    <row r="147" spans="1:23" s="185" customFormat="1" ht="69" customHeight="1">
+    <row r="147" spans="1:23" s="185" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="116">
         <v>94</v>
       </c>
@@ -9456,7 +9506,7 @@
       <c r="V147" s="187"/>
       <c r="W147" s="187"/>
     </row>
-    <row r="148" spans="1:23" s="185" customFormat="1" ht="73.5" customHeight="1">
+    <row r="148" spans="1:23" s="185" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="116">
         <v>95</v>
       </c>
@@ -9490,13 +9540,13 @@
         <v>0</v>
       </c>
       <c r="T148" s="133"/>
-      <c r="U148" s="267" t="s">
+      <c r="U148" s="271" t="s">
         <v>206</v>
       </c>
       <c r="V148" s="187"/>
       <c r="W148" s="187"/>
     </row>
-    <row r="149" spans="1:23" s="185" customFormat="1" ht="47.25" customHeight="1">
+    <row r="149" spans="1:23" s="185" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="116">
         <v>96</v>
       </c>
@@ -9538,11 +9588,11 @@
         <v>0</v>
       </c>
       <c r="T149" s="133"/>
-      <c r="U149" s="268"/>
+      <c r="U149" s="272"/>
       <c r="V149" s="160"/>
       <c r="W149" s="160"/>
     </row>
-    <row r="150" spans="1:23" s="185" customFormat="1" ht="46.5" customHeight="1">
+    <row r="150" spans="1:23" s="185" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="116">
         <v>97</v>
       </c>
@@ -9576,11 +9626,11 @@
         <v>0</v>
       </c>
       <c r="T150" s="133"/>
-      <c r="U150" s="269"/>
+      <c r="U150" s="273"/>
       <c r="V150" s="187"/>
       <c r="W150" s="187"/>
     </row>
-    <row r="151" spans="1:23" s="185" customFormat="1" ht="65.25" customHeight="1">
+    <row r="151" spans="1:23" s="185" customFormat="1" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="116">
         <v>98</v>
       </c>
@@ -9614,13 +9664,13 @@
         <v>0</v>
       </c>
       <c r="T151" s="133"/>
-      <c r="U151" s="267" t="s">
+      <c r="U151" s="271" t="s">
         <v>209</v>
       </c>
       <c r="V151" s="160"/>
       <c r="W151" s="160"/>
     </row>
-    <row r="152" spans="1:23" s="185" customFormat="1" ht="45" customHeight="1">
+    <row r="152" spans="1:23" s="185" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="116">
         <v>99</v>
       </c>
@@ -9662,11 +9712,11 @@
         <v>0</v>
       </c>
       <c r="T152" s="133"/>
-      <c r="U152" s="268"/>
+      <c r="U152" s="272"/>
       <c r="V152" s="160"/>
       <c r="W152" s="160"/>
     </row>
-    <row r="153" spans="1:23" s="185" customFormat="1" ht="46.5" customHeight="1">
+    <row r="153" spans="1:23" s="185" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="116">
         <v>100</v>
       </c>
@@ -9700,11 +9750,11 @@
         <v>0</v>
       </c>
       <c r="T153" s="133"/>
-      <c r="U153" s="269"/>
+      <c r="U153" s="273"/>
       <c r="V153" s="160"/>
       <c r="W153" s="160"/>
     </row>
-    <row r="154" spans="1:23" s="185" customFormat="1" ht="64.5" customHeight="1">
+    <row r="154" spans="1:23" s="185" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="116">
         <v>101</v>
       </c>
@@ -9738,13 +9788,13 @@
         <v>0</v>
       </c>
       <c r="T154" s="133"/>
-      <c r="U154" s="267" t="s">
+      <c r="U154" s="271" t="s">
         <v>211</v>
       </c>
       <c r="V154" s="160"/>
       <c r="W154" s="160"/>
     </row>
-    <row r="155" spans="1:23" s="185" customFormat="1" ht="48.75" customHeight="1">
+    <row r="155" spans="1:23" s="185" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="116">
         <v>102</v>
       </c>
@@ -9788,11 +9838,11 @@
       <c r="T155" s="133">
         <v>100</v>
       </c>
-      <c r="U155" s="268"/>
+      <c r="U155" s="272"/>
       <c r="V155" s="160"/>
       <c r="W155" s="160"/>
     </row>
-    <row r="156" spans="1:23" s="185" customFormat="1" ht="45" customHeight="1">
+    <row r="156" spans="1:23" s="185" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="116">
         <v>103</v>
       </c>
@@ -9826,11 +9876,11 @@
         <v>0</v>
       </c>
       <c r="T156" s="133"/>
-      <c r="U156" s="269"/>
+      <c r="U156" s="273"/>
       <c r="V156" s="160"/>
       <c r="W156" s="160"/>
     </row>
-    <row r="157" spans="1:23" s="185" customFormat="1" ht="54.75" customHeight="1">
+    <row r="157" spans="1:23" s="185" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="116">
         <v>104</v>
       </c>
@@ -9864,13 +9914,13 @@
         <v>0</v>
       </c>
       <c r="T157" s="133"/>
-      <c r="U157" s="267" t="s">
+      <c r="U157" s="271" t="s">
         <v>214</v>
       </c>
       <c r="V157" s="160"/>
       <c r="W157" s="160"/>
     </row>
-    <row r="158" spans="1:23" s="185" customFormat="1" ht="41.25" customHeight="1">
+    <row r="158" spans="1:23" s="185" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="116">
         <v>105</v>
       </c>
@@ -9912,11 +9962,11 @@
         <v>0</v>
       </c>
       <c r="T158" s="133"/>
-      <c r="U158" s="268"/>
+      <c r="U158" s="272"/>
       <c r="V158" s="160"/>
       <c r="W158" s="160"/>
     </row>
-    <row r="159" spans="1:23" s="185" customFormat="1" ht="41.25" customHeight="1">
+    <row r="159" spans="1:23" s="185" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="116">
         <v>106</v>
       </c>
@@ -9950,11 +10000,11 @@
         <v>0</v>
       </c>
       <c r="T159" s="133"/>
-      <c r="U159" s="269"/>
+      <c r="U159" s="273"/>
       <c r="V159" s="187"/>
       <c r="W159" s="187"/>
     </row>
-    <row r="160" spans="1:23" s="185" customFormat="1" ht="51" customHeight="1">
+    <row r="160" spans="1:23" s="185" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="116">
         <v>107</v>
       </c>
@@ -9988,13 +10038,13 @@
         <v>0</v>
       </c>
       <c r="T160" s="133"/>
-      <c r="U160" s="267" t="s">
+      <c r="U160" s="271" t="s">
         <v>216</v>
       </c>
       <c r="V160" s="160"/>
       <c r="W160" s="160"/>
     </row>
-    <row r="161" spans="1:23" s="185" customFormat="1" ht="42" customHeight="1">
+    <row r="161" spans="1:23" s="185" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="116">
         <v>108</v>
       </c>
@@ -10038,11 +10088,11 @@
       <c r="T161" s="133">
         <v>100</v>
       </c>
-      <c r="U161" s="268"/>
+      <c r="U161" s="272"/>
       <c r="V161" s="187"/>
       <c r="W161" s="187"/>
     </row>
-    <row r="162" spans="1:23" s="185" customFormat="1" ht="42" customHeight="1">
+    <row r="162" spans="1:23" s="185" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="116">
         <v>109</v>
       </c>
@@ -10076,11 +10126,11 @@
         <v>0</v>
       </c>
       <c r="T162" s="133"/>
-      <c r="U162" s="269"/>
+      <c r="U162" s="273"/>
       <c r="V162" s="187"/>
       <c r="W162" s="187"/>
     </row>
-    <row r="163" spans="1:23" s="185" customFormat="1" ht="66.75" customHeight="1">
+    <row r="163" spans="1:23" s="185" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="116">
         <v>110</v>
       </c>
@@ -10114,13 +10164,13 @@
         <v>0</v>
       </c>
       <c r="T163" s="133"/>
-      <c r="U163" s="267" t="s">
+      <c r="U163" s="271" t="s">
         <v>218</v>
       </c>
       <c r="V163" s="160"/>
       <c r="W163" s="160"/>
     </row>
-    <row r="164" spans="1:23" s="185" customFormat="1" ht="44.25" customHeight="1">
+    <row r="164" spans="1:23" s="185" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="116">
         <v>111</v>
       </c>
@@ -10164,11 +10214,11 @@
       <c r="T164" s="133">
         <v>100</v>
       </c>
-      <c r="U164" s="268"/>
+      <c r="U164" s="272"/>
       <c r="V164" s="187"/>
       <c r="W164" s="187"/>
     </row>
-    <row r="165" spans="1:23" s="185" customFormat="1" ht="36.75" customHeight="1">
+    <row r="165" spans="1:23" s="185" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="116">
         <v>112</v>
       </c>
@@ -10202,11 +10252,11 @@
         <v>0</v>
       </c>
       <c r="T165" s="133"/>
-      <c r="U165" s="269"/>
+      <c r="U165" s="273"/>
       <c r="V165" s="187"/>
       <c r="W165" s="187"/>
     </row>
-    <row r="166" spans="1:23" s="185" customFormat="1" ht="67.5" customHeight="1">
+    <row r="166" spans="1:23" s="185" customFormat="1" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="116">
         <v>113</v>
       </c>
@@ -10240,13 +10290,13 @@
         <v>0</v>
       </c>
       <c r="T166" s="133"/>
-      <c r="U166" s="267" t="s">
+      <c r="U166" s="271" t="s">
         <v>220</v>
       </c>
       <c r="V166" s="160"/>
       <c r="W166" s="160"/>
     </row>
-    <row r="167" spans="1:23" s="185" customFormat="1" ht="41.25" customHeight="1">
+    <row r="167" spans="1:23" s="185" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="116">
         <v>114</v>
       </c>
@@ -10290,11 +10340,11 @@
       <c r="T167" s="133">
         <v>100</v>
       </c>
-      <c r="U167" s="268"/>
+      <c r="U167" s="272"/>
       <c r="V167" s="187"/>
       <c r="W167" s="187"/>
     </row>
-    <row r="168" spans="1:23" s="185" customFormat="1" ht="41.25" customHeight="1">
+    <row r="168" spans="1:23" s="185" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="116">
         <v>115</v>
       </c>
@@ -10328,11 +10378,11 @@
         <v>0</v>
       </c>
       <c r="T168" s="133"/>
-      <c r="U168" s="269"/>
+      <c r="U168" s="273"/>
       <c r="V168" s="187"/>
       <c r="W168" s="187"/>
     </row>
-    <row r="169" spans="1:23" s="185" customFormat="1" ht="65.25" customHeight="1">
+    <row r="169" spans="1:23" s="185" customFormat="1" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="116">
         <v>116</v>
       </c>
@@ -10366,13 +10416,13 @@
         <v>0</v>
       </c>
       <c r="T169" s="133"/>
-      <c r="U169" s="267" t="s">
+      <c r="U169" s="271" t="s">
         <v>222</v>
       </c>
       <c r="V169" s="160"/>
       <c r="W169" s="160"/>
     </row>
-    <row r="170" spans="1:23" s="185" customFormat="1" ht="39.75" customHeight="1">
+    <row r="170" spans="1:23" s="185" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="116">
         <v>117</v>
       </c>
@@ -10416,11 +10466,11 @@
       <c r="T170" s="133">
         <v>100</v>
       </c>
-      <c r="U170" s="268"/>
+      <c r="U170" s="272"/>
       <c r="V170" s="187"/>
       <c r="W170" s="187"/>
     </row>
-    <row r="171" spans="1:23" s="188" customFormat="1" ht="39.75" customHeight="1">
+    <row r="171" spans="1:23" s="188" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="116">
         <v>118</v>
       </c>
@@ -10454,11 +10504,11 @@
         <v>0</v>
       </c>
       <c r="T171" s="133"/>
-      <c r="U171" s="269"/>
+      <c r="U171" s="273"/>
       <c r="V171" s="160"/>
       <c r="W171" s="160"/>
     </row>
-    <row r="172" spans="1:23" s="185" customFormat="1" ht="45" customHeight="1">
+    <row r="172" spans="1:23" s="185" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="116">
         <v>119</v>
       </c>
@@ -10492,13 +10542,13 @@
         <v>0</v>
       </c>
       <c r="T172" s="133"/>
-      <c r="U172" s="267" t="s">
+      <c r="U172" s="271" t="s">
         <v>224</v>
       </c>
       <c r="V172" s="160"/>
       <c r="W172" s="160"/>
     </row>
-    <row r="173" spans="1:23" s="185" customFormat="1" ht="45" customHeight="1">
+    <row r="173" spans="1:23" s="185" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="116">
         <v>120</v>
       </c>
@@ -10542,11 +10592,11 @@
       <c r="T173" s="133">
         <v>100</v>
       </c>
-      <c r="U173" s="268"/>
+      <c r="U173" s="272"/>
       <c r="V173" s="160"/>
       <c r="W173" s="160"/>
     </row>
-    <row r="174" spans="1:23" s="185" customFormat="1" ht="45" customHeight="1">
+    <row r="174" spans="1:23" s="185" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="116">
         <v>121</v>
       </c>
@@ -10580,11 +10630,11 @@
         <v>0</v>
       </c>
       <c r="T174" s="133"/>
-      <c r="U174" s="269"/>
+      <c r="U174" s="273"/>
       <c r="V174" s="160"/>
       <c r="W174" s="160"/>
     </row>
-    <row r="175" spans="1:23" s="185" customFormat="1" ht="73.5" customHeight="1">
+    <row r="175" spans="1:23" s="185" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="116">
         <v>122</v>
       </c>
@@ -10618,13 +10668,13 @@
         <v>0</v>
       </c>
       <c r="T175" s="133"/>
-      <c r="U175" s="267" t="s">
+      <c r="U175" s="271" t="s">
         <v>226</v>
       </c>
       <c r="V175" s="160"/>
       <c r="W175" s="160"/>
     </row>
-    <row r="176" spans="1:23" s="185" customFormat="1" ht="45" customHeight="1">
+    <row r="176" spans="1:23" s="185" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="116">
         <v>123</v>
       </c>
@@ -10668,11 +10718,11 @@
       <c r="T176" s="133">
         <v>100</v>
       </c>
-      <c r="U176" s="268"/>
+      <c r="U176" s="272"/>
       <c r="V176" s="160"/>
       <c r="W176" s="160"/>
     </row>
-    <row r="177" spans="1:23" s="185" customFormat="1" ht="45" customHeight="1">
+    <row r="177" spans="1:23" s="185" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="116">
         <v>124</v>
       </c>
@@ -10706,11 +10756,11 @@
         <v>0</v>
       </c>
       <c r="T177" s="133"/>
-      <c r="U177" s="269"/>
+      <c r="U177" s="273"/>
       <c r="V177" s="160"/>
       <c r="W177" s="160"/>
     </row>
-    <row r="178" spans="1:23" s="185" customFormat="1" ht="45" customHeight="1">
+    <row r="178" spans="1:23" s="185" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="116">
         <v>125</v>
       </c>
@@ -10744,13 +10794,13 @@
         <v>0</v>
       </c>
       <c r="T178" s="133"/>
-      <c r="U178" s="267" t="s">
+      <c r="U178" s="271" t="s">
         <v>228</v>
       </c>
       <c r="V178" s="160"/>
       <c r="W178" s="160"/>
     </row>
-    <row r="179" spans="1:23" s="185" customFormat="1" ht="45" customHeight="1">
+    <row r="179" spans="1:23" s="185" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="116">
         <v>126</v>
       </c>
@@ -10794,11 +10844,11 @@
       <c r="T179" s="133">
         <v>100</v>
       </c>
-      <c r="U179" s="268"/>
+      <c r="U179" s="272"/>
       <c r="V179" s="160"/>
       <c r="W179" s="160"/>
     </row>
-    <row r="180" spans="1:23" s="185" customFormat="1" ht="45" customHeight="1">
+    <row r="180" spans="1:23" s="185" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="116">
         <v>127</v>
       </c>
@@ -10832,11 +10882,11 @@
         <v>0</v>
       </c>
       <c r="T180" s="133"/>
-      <c r="U180" s="269"/>
+      <c r="U180" s="273"/>
       <c r="V180" s="160"/>
       <c r="W180" s="160"/>
     </row>
-    <row r="181" spans="1:23" s="185" customFormat="1" ht="72" customHeight="1">
+    <row r="181" spans="1:23" s="185" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="116">
         <v>128</v>
       </c>
@@ -10870,13 +10920,13 @@
         <v>0</v>
       </c>
       <c r="T181" s="133"/>
-      <c r="U181" s="267" t="s">
+      <c r="U181" s="271" t="s">
         <v>230</v>
       </c>
       <c r="V181" s="160"/>
       <c r="W181" s="160"/>
     </row>
-    <row r="182" spans="1:23" s="185" customFormat="1" ht="45" customHeight="1">
+    <row r="182" spans="1:23" s="185" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="116">
         <v>129</v>
       </c>
@@ -10920,11 +10970,11 @@
       <c r="T182" s="133">
         <v>100</v>
       </c>
-      <c r="U182" s="268"/>
+      <c r="U182" s="272"/>
       <c r="V182" s="160"/>
       <c r="W182" s="160"/>
     </row>
-    <row r="183" spans="1:23" s="185" customFormat="1" ht="45.75" customHeight="1">
+    <row r="183" spans="1:23" s="185" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="116">
         <v>130</v>
       </c>
@@ -10958,11 +11008,11 @@
         <v>0</v>
       </c>
       <c r="T183" s="133"/>
-      <c r="U183" s="269"/>
+      <c r="U183" s="273"/>
       <c r="V183" s="160"/>
       <c r="W183" s="160"/>
     </row>
-    <row r="184" spans="1:23" s="185" customFormat="1" ht="14.25" customHeight="1">
+    <row r="184" spans="1:23" s="185" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="116"/>
       <c r="B184" s="227"/>
       <c r="C184" s="213"/>
@@ -10987,7 +11037,7 @@
       <c r="V184" s="187"/>
       <c r="W184" s="187"/>
     </row>
-    <row r="185" spans="1:23" s="127" customFormat="1" ht="65.25" customHeight="1">
+    <row r="185" spans="1:23" s="127" customFormat="1" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="116"/>
       <c r="B185" s="227" t="s">
         <v>231</v>
@@ -11028,7 +11078,7 @@
       <c r="V185" s="187"/>
       <c r="W185" s="187"/>
     </row>
-    <row r="186" spans="1:23" s="185" customFormat="1" ht="45">
+    <row r="186" spans="1:23" s="185" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A186" s="116">
         <v>131</v>
       </c>
@@ -11051,11 +11101,11 @@
       <c r="H186" s="132" t="s">
         <v>235</v>
       </c>
-      <c r="I186" s="280" t="s">
+      <c r="I186" s="268" t="s">
         <v>237</v>
       </c>
-      <c r="J186" s="281"/>
-      <c r="K186" s="282"/>
+      <c r="J186" s="269"/>
+      <c r="K186" s="270"/>
       <c r="L186" s="132"/>
       <c r="M186" s="132"/>
       <c r="N186" s="132" t="s">
@@ -11080,7 +11130,7 @@
       <c r="V186" s="187"/>
       <c r="W186" s="187"/>
     </row>
-    <row r="187" spans="1:23" s="185" customFormat="1" ht="45">
+    <row r="187" spans="1:23" s="185" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A187" s="116">
         <v>132</v>
       </c>
@@ -11097,9 +11147,9 @@
       <c r="F187" s="132"/>
       <c r="G187" s="132"/>
       <c r="H187" s="132"/>
-      <c r="I187" s="280"/>
-      <c r="J187" s="281"/>
-      <c r="K187" s="282"/>
+      <c r="I187" s="268"/>
+      <c r="J187" s="269"/>
+      <c r="K187" s="270"/>
       <c r="L187" s="132"/>
       <c r="M187" s="132"/>
       <c r="N187" s="132" t="s">
@@ -11120,7 +11170,7 @@
       <c r="V187" s="187"/>
       <c r="W187" s="187"/>
     </row>
-    <row r="188" spans="1:23" s="185" customFormat="1" ht="45">
+    <row r="188" spans="1:23" s="185" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A188" s="116">
         <v>133</v>
       </c>
@@ -11137,9 +11187,9 @@
       <c r="F188" s="132"/>
       <c r="G188" s="132"/>
       <c r="H188" s="132"/>
-      <c r="I188" s="280"/>
-      <c r="J188" s="281"/>
-      <c r="K188" s="282"/>
+      <c r="I188" s="268"/>
+      <c r="J188" s="269"/>
+      <c r="K188" s="270"/>
       <c r="L188" s="132"/>
       <c r="M188" s="132"/>
       <c r="N188" s="132" t="s">
@@ -11160,7 +11210,7 @@
       <c r="V188" s="187"/>
       <c r="W188" s="187"/>
     </row>
-    <row r="189" spans="1:23" s="185" customFormat="1" ht="45">
+    <row r="189" spans="1:23" s="185" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A189" s="128">
         <v>134</v>
       </c>
@@ -11177,9 +11227,9 @@
       <c r="F189" s="132"/>
       <c r="G189" s="132"/>
       <c r="H189" s="132"/>
-      <c r="I189" s="280"/>
-      <c r="J189" s="281"/>
-      <c r="K189" s="282"/>
+      <c r="I189" s="268"/>
+      <c r="J189" s="269"/>
+      <c r="K189" s="270"/>
       <c r="L189" s="132"/>
       <c r="M189" s="132"/>
       <c r="N189" s="132" t="s">
@@ -11200,7 +11250,7 @@
       <c r="V189" s="187"/>
       <c r="W189" s="187"/>
     </row>
-    <row r="190" spans="1:23">
+    <row r="190" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A190" s="189"/>
       <c r="B190" s="241"/>
       <c r="C190" s="222"/>
@@ -11225,7 +11275,7 @@
       <c r="V190" s="197"/>
       <c r="W190" s="197"/>
     </row>
-    <row r="192" spans="1:23" ht="15" customHeight="1">
+    <row r="192" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C192" s="65"/>
       <c r="D192" s="65"/>
       <c r="E192" s="63"/>
@@ -11245,7 +11295,7 @@
       <c r="V192"/>
       <c r="W192"/>
     </row>
-    <row r="193" spans="1:23" ht="15" customHeight="1">
+    <row r="193" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C193" s="65"/>
       <c r="D193" s="65"/>
       <c r="E193" s="63"/>
@@ -11265,7 +11315,7 @@
       <c r="V193"/>
       <c r="W193"/>
     </row>
-    <row r="194" spans="1:23">
+    <row r="194" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C194" s="65"/>
       <c r="D194" s="65"/>
       <c r="E194" s="63"/>
@@ -11285,7 +11335,7 @@
       <c r="V194"/>
       <c r="W194"/>
     </row>
-    <row r="195" spans="1:23">
+    <row r="195" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C195" s="65"/>
       <c r="D195" s="65"/>
       <c r="E195" s="63"/>
@@ -11305,7 +11355,7 @@
       <c r="V195"/>
       <c r="W195"/>
     </row>
-    <row r="196" spans="1:23">
+    <row r="196" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C196" s="65"/>
       <c r="D196" s="65"/>
       <c r="E196" s="63"/>
@@ -11325,7 +11375,7 @@
       <c r="V196"/>
       <c r="W196"/>
     </row>
-    <row r="197" spans="1:23">
+    <row r="197" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C197" s="65"/>
       <c r="D197" s="65"/>
       <c r="E197" s="63"/>
@@ -11345,7 +11395,7 @@
       <c r="V197"/>
       <c r="W197"/>
     </row>
-    <row r="198" spans="1:23" s="67" customFormat="1">
+    <row r="198" spans="1:23" s="67" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A198"/>
       <c r="B198" s="200"/>
       <c r="C198" s="65"/>
@@ -11370,7 +11420,7 @@
       <c r="V198"/>
       <c r="W198"/>
     </row>
-    <row r="199" spans="1:23" s="67" customFormat="1" ht="15.75" customHeight="1">
+    <row r="199" spans="1:23" s="67" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199"/>
       <c r="B199" s="200"/>
       <c r="C199" s="65"/>
@@ -11395,7 +11445,7 @@
       <c r="V199"/>
       <c r="W199"/>
     </row>
-    <row r="200" spans="1:23" s="67" customFormat="1" ht="15.75" customHeight="1">
+    <row r="200" spans="1:23" s="67" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200"/>
       <c r="B200" s="200"/>
       <c r="C200" s="65"/>
@@ -11420,7 +11470,7 @@
       <c r="V200"/>
       <c r="W200"/>
     </row>
-    <row r="201" spans="1:23" s="67" customFormat="1" ht="15.75" customHeight="1">
+    <row r="201" spans="1:23" s="67" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201"/>
       <c r="B201" s="200"/>
       <c r="C201" s="65"/>
@@ -11445,11 +11495,11 @@
       <c r="V201"/>
       <c r="W201"/>
     </row>
-    <row r="202" spans="1:23">
+    <row r="202" spans="1:23" x14ac:dyDescent="0.25">
       <c r="F202" s="198"/>
       <c r="G202" s="200"/>
     </row>
-    <row r="207" spans="1:23" s="67" customFormat="1">
+    <row r="207" spans="1:23" s="67" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A207"/>
       <c r="B207" s="200"/>
       <c r="C207" s="61"/>
@@ -11474,7 +11524,7 @@
       <c r="V207" s="68"/>
       <c r="W207" s="68"/>
     </row>
-    <row r="208" spans="1:23" s="67" customFormat="1">
+    <row r="208" spans="1:23" s="67" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A208"/>
       <c r="B208" s="200"/>
       <c r="C208" s="61"/>
@@ -11499,40 +11549,64 @@
       <c r="V208" s="68"/>
       <c r="W208" s="68"/>
     </row>
-    <row r="209" spans="6:7">
+    <row r="209" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F209" s="198"/>
       <c r="G209"/>
     </row>
-    <row r="210" spans="6:7">
+    <row r="210" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F210" s="198"/>
       <c r="G210" s="199"/>
     </row>
-    <row r="211" spans="6:7">
+    <row r="211" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F211" s="198"/>
       <c r="G211"/>
     </row>
-    <row r="212" spans="6:7">
+    <row r="212" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F212" s="198"/>
       <c r="G212"/>
     </row>
-    <row r="213" spans="6:7">
+    <row r="213" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F213" s="198"/>
       <c r="G213"/>
     </row>
   </sheetData>
   <mergeCells count="68">
-    <mergeCell ref="W5:W8"/>
-    <mergeCell ref="V5:V8"/>
-    <mergeCell ref="A1:W1"/>
-    <mergeCell ref="A2:W2"/>
-    <mergeCell ref="A3:W3"/>
-    <mergeCell ref="H5:H8"/>
-    <mergeCell ref="R5:T6"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="C5:C8"/>
-    <mergeCell ref="D5:D8"/>
-    <mergeCell ref="E5:E8"/>
+    <mergeCell ref="I5:M6"/>
+    <mergeCell ref="N5:N8"/>
+    <mergeCell ref="P5:P8"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="U178:U180"/>
+    <mergeCell ref="U181:U183"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="U160:U162"/>
+    <mergeCell ref="U163:U165"/>
+    <mergeCell ref="U166:U168"/>
+    <mergeCell ref="U169:U171"/>
+    <mergeCell ref="U172:U174"/>
+    <mergeCell ref="U175:U177"/>
+    <mergeCell ref="U132:U134"/>
+    <mergeCell ref="U135:U137"/>
+    <mergeCell ref="U148:U150"/>
+    <mergeCell ref="U151:U153"/>
+    <mergeCell ref="U154:U156"/>
+    <mergeCell ref="U86:U91"/>
+    <mergeCell ref="U94:U96"/>
+    <mergeCell ref="U97:U99"/>
+    <mergeCell ref="U100:U102"/>
+    <mergeCell ref="U157:U159"/>
+    <mergeCell ref="U114:U116"/>
+    <mergeCell ref="U117:U119"/>
+    <mergeCell ref="U120:U122"/>
+    <mergeCell ref="U123:U125"/>
+    <mergeCell ref="U126:U128"/>
+    <mergeCell ref="U129:U131"/>
+    <mergeCell ref="U66:U68"/>
+    <mergeCell ref="U69:U71"/>
+    <mergeCell ref="U72:U74"/>
+    <mergeCell ref="U77:U79"/>
+    <mergeCell ref="U80:U82"/>
     <mergeCell ref="I187:K187"/>
     <mergeCell ref="I188:K188"/>
     <mergeCell ref="I189:K189"/>
@@ -11549,49 +11623,26 @@
     <mergeCell ref="U111:U113"/>
     <mergeCell ref="U54:U56"/>
     <mergeCell ref="U60:U62"/>
-    <mergeCell ref="U66:U68"/>
-    <mergeCell ref="U69:U71"/>
-    <mergeCell ref="U72:U74"/>
-    <mergeCell ref="U77:U79"/>
-    <mergeCell ref="U80:U82"/>
-    <mergeCell ref="U86:U91"/>
-    <mergeCell ref="U94:U96"/>
-    <mergeCell ref="U97:U99"/>
-    <mergeCell ref="U100:U102"/>
-    <mergeCell ref="U157:U159"/>
-    <mergeCell ref="U114:U116"/>
-    <mergeCell ref="U117:U119"/>
-    <mergeCell ref="U120:U122"/>
-    <mergeCell ref="U123:U125"/>
-    <mergeCell ref="U126:U128"/>
-    <mergeCell ref="U129:U131"/>
-    <mergeCell ref="U178:U180"/>
-    <mergeCell ref="U181:U183"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="U160:U162"/>
-    <mergeCell ref="U163:U165"/>
-    <mergeCell ref="U166:U168"/>
-    <mergeCell ref="U169:U171"/>
-    <mergeCell ref="U172:U174"/>
-    <mergeCell ref="U175:U177"/>
-    <mergeCell ref="U132:U134"/>
-    <mergeCell ref="U135:U137"/>
-    <mergeCell ref="U148:U150"/>
-    <mergeCell ref="U151:U153"/>
-    <mergeCell ref="U154:U156"/>
+    <mergeCell ref="W5:W8"/>
+    <mergeCell ref="V5:V8"/>
+    <mergeCell ref="A1:W1"/>
+    <mergeCell ref="A2:W2"/>
+    <mergeCell ref="A3:W3"/>
+    <mergeCell ref="H5:H8"/>
+    <mergeCell ref="R5:T6"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="C5:C8"/>
+    <mergeCell ref="D5:D8"/>
+    <mergeCell ref="E5:E8"/>
     <mergeCell ref="Q5:Q7"/>
     <mergeCell ref="U5:U8"/>
     <mergeCell ref="F5:G8"/>
     <mergeCell ref="O5:O8"/>
-    <mergeCell ref="I5:M6"/>
-    <mergeCell ref="N5:N8"/>
-    <mergeCell ref="P5:P8"/>
-    <mergeCell ref="R7:S7"/>
   </mergeCells>
-  <pageMargins left="0.39370078740157499" right="0.196850393700787" top="0.78740157480314998" bottom="0.59055118110236204" header="0.31496062992126" footer="0.27559055118110198"/>
-  <pageSetup paperSize="8" scale="39" orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0" right="0" top="0.78740157480314965" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.27559055118110237"/>
+  <pageSetup paperSize="10001" scale="36" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="145" max="34" man="1"/>
   </rowBreaks>
@@ -11599,19 +11650,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:II15"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="80" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.7109375" style="36" customWidth="1"/>
     <col min="2" max="2" width="17.42578125" style="36" customWidth="1"/>
@@ -11640,33 +11692,33 @@
     <col min="244" max="16384" width="9" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:243" ht="23.25">
-      <c r="A1" s="300" t="s">
+    <row r="1" spans="1:243" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="313" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="300"/>
-      <c r="C1" s="300"/>
-      <c r="D1" s="300"/>
-      <c r="E1" s="300"/>
-      <c r="F1" s="300"/>
-      <c r="G1" s="300"/>
-      <c r="H1" s="300"/>
-      <c r="I1" s="300"/>
-      <c r="J1" s="300"/>
-      <c r="K1" s="300"/>
-      <c r="L1" s="300"/>
-      <c r="M1" s="300"/>
-      <c r="N1" s="300"/>
-      <c r="O1" s="300"/>
-      <c r="P1" s="300"/>
-      <c r="Q1" s="300"/>
-      <c r="R1" s="300"/>
-      <c r="S1" s="300"/>
-      <c r="T1" s="300"/>
-      <c r="U1" s="300"/>
-      <c r="V1" s="300"/>
-    </row>
-    <row r="2" spans="1:243" ht="18.75">
+      <c r="B1" s="313"/>
+      <c r="C1" s="313"/>
+      <c r="D1" s="313"/>
+      <c r="E1" s="313"/>
+      <c r="F1" s="313"/>
+      <c r="G1" s="313"/>
+      <c r="H1" s="313"/>
+      <c r="I1" s="313"/>
+      <c r="J1" s="313"/>
+      <c r="K1" s="313"/>
+      <c r="L1" s="313"/>
+      <c r="M1" s="313"/>
+      <c r="N1" s="313"/>
+      <c r="O1" s="313"/>
+      <c r="P1" s="313"/>
+      <c r="Q1" s="313"/>
+      <c r="R1" s="313"/>
+      <c r="S1" s="313"/>
+      <c r="T1" s="313"/>
+      <c r="U1" s="313"/>
+      <c r="V1" s="313"/>
+    </row>
+    <row r="2" spans="1:243" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
         <v>12</v>
       </c>
@@ -11692,7 +11744,7 @@
       <c r="U2" s="20"/>
       <c r="V2" s="20"/>
     </row>
-    <row r="3" spans="1:243" ht="18.75">
+    <row r="3" spans="1:243" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>21</v>
       </c>
@@ -11718,7 +11770,7 @@
       <c r="U3" s="20"/>
       <c r="V3" s="20"/>
     </row>
-    <row r="4" spans="1:243" ht="16.5" thickBot="1">
+    <row r="4" spans="1:243" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="21"/>
       <c r="B4" s="21"/>
       <c r="C4" s="21"/>
@@ -11742,58 +11794,58 @@
       <c r="U4" s="20"/>
       <c r="V4" s="20"/>
     </row>
-    <row r="5" spans="1:243" s="40" customFormat="1" ht="16.5" customHeight="1" thickTop="1">
-      <c r="A5" s="301" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="310" t="s">
+    <row r="5" spans="1:243" s="40" customFormat="1" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="314" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="293" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="311"/>
-      <c r="D5" s="304" t="s">
+      <c r="C5" s="294"/>
+      <c r="D5" s="317" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="305"/>
-      <c r="F5" s="297" t="s">
+      <c r="E5" s="318"/>
+      <c r="F5" s="312" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="306" t="s">
+      <c r="G5" s="297" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="306" t="s">
+      <c r="H5" s="297" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="318" t="s">
+      <c r="I5" s="303" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="319"/>
-      <c r="K5" s="319"/>
-      <c r="L5" s="319"/>
-      <c r="M5" s="320"/>
-      <c r="N5" s="306" t="s">
+      <c r="J5" s="304"/>
+      <c r="K5" s="304"/>
+      <c r="L5" s="304"/>
+      <c r="M5" s="305"/>
+      <c r="N5" s="297" t="s">
         <v>27</v>
       </c>
-      <c r="O5" s="306" t="s">
+      <c r="O5" s="297" t="s">
         <v>26</v>
       </c>
-      <c r="P5" s="297" t="s">
+      <c r="P5" s="312" t="s">
         <v>9</v>
       </c>
-      <c r="Q5" s="306" t="s">
+      <c r="Q5" s="297" t="s">
         <v>28</v>
       </c>
-      <c r="R5" s="310" t="s">
+      <c r="R5" s="293" t="s">
         <v>31</v>
       </c>
-      <c r="S5" s="317"/>
-      <c r="T5" s="311"/>
-      <c r="U5" s="306" t="s">
+      <c r="S5" s="302"/>
+      <c r="T5" s="294"/>
+      <c r="U5" s="297" t="s">
         <v>29</v>
       </c>
-      <c r="V5" s="301" t="s">
+      <c r="V5" s="314" t="s">
         <v>30</v>
       </c>
-      <c r="W5" s="306" t="s">
+      <c r="W5" s="297" t="s">
         <v>41</v>
       </c>
       <c r="X5" s="38"/>
@@ -12017,19 +12069,19 @@
       <c r="IH5" s="38"/>
       <c r="II5" s="38"/>
     </row>
-    <row r="6" spans="1:243" s="40" customFormat="1" ht="37.5" customHeight="1">
-      <c r="A6" s="302"/>
-      <c r="B6" s="312"/>
-      <c r="C6" s="313"/>
-      <c r="D6" s="302" t="s">
+    <row r="6" spans="1:243" s="40" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="315"/>
+      <c r="B6" s="295"/>
+      <c r="C6" s="296"/>
+      <c r="D6" s="315" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="298" t="s">
+      <c r="E6" s="306" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="298"/>
-      <c r="G6" s="307"/>
-      <c r="H6" s="307"/>
+      <c r="F6" s="306"/>
+      <c r="G6" s="298"/>
+      <c r="H6" s="298"/>
       <c r="I6" s="41" t="s">
         <v>6</v>
       </c>
@@ -12039,26 +12091,26 @@
       <c r="K6" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="298" t="s">
+      <c r="L6" s="306" t="s">
         <v>4</v>
       </c>
-      <c r="M6" s="298" t="s">
+      <c r="M6" s="306" t="s">
         <v>36</v>
       </c>
-      <c r="N6" s="307"/>
-      <c r="O6" s="307"/>
-      <c r="P6" s="298"/>
-      <c r="Q6" s="307"/>
-      <c r="R6" s="314" t="s">
+      <c r="N6" s="298"/>
+      <c r="O6" s="298"/>
+      <c r="P6" s="306"/>
+      <c r="Q6" s="298"/>
+      <c r="R6" s="299" t="s">
         <v>32</v>
       </c>
-      <c r="S6" s="315"/>
+      <c r="S6" s="300"/>
       <c r="T6" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="U6" s="307"/>
-      <c r="V6" s="302"/>
-      <c r="W6" s="307"/>
+      <c r="U6" s="298"/>
+      <c r="V6" s="315"/>
+      <c r="W6" s="298"/>
       <c r="X6" s="38"/>
       <c r="Y6" s="38"/>
       <c r="Z6" s="38"/>
@@ -12280,15 +12332,15 @@
       <c r="IH6" s="38"/>
       <c r="II6" s="38"/>
     </row>
-    <row r="7" spans="1:243" s="40" customFormat="1" ht="20.25" customHeight="1" thickBot="1">
-      <c r="A7" s="303"/>
-      <c r="B7" s="312"/>
-      <c r="C7" s="313"/>
-      <c r="D7" s="303"/>
-      <c r="E7" s="299"/>
-      <c r="F7" s="299"/>
-      <c r="G7" s="307"/>
-      <c r="H7" s="316"/>
+    <row r="7" spans="1:243" s="40" customFormat="1" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="316"/>
+      <c r="B7" s="295"/>
+      <c r="C7" s="296"/>
+      <c r="D7" s="316"/>
+      <c r="E7" s="307"/>
+      <c r="F7" s="307"/>
+      <c r="G7" s="298"/>
+      <c r="H7" s="301"/>
       <c r="I7" s="43" t="s">
         <v>5</v>
       </c>
@@ -12298,12 +12350,12 @@
       <c r="K7" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="L7" s="299"/>
-      <c r="M7" s="299"/>
-      <c r="N7" s="307"/>
-      <c r="O7" s="307"/>
-      <c r="P7" s="299"/>
-      <c r="Q7" s="307"/>
+      <c r="L7" s="307"/>
+      <c r="M7" s="307"/>
+      <c r="N7" s="298"/>
+      <c r="O7" s="298"/>
+      <c r="P7" s="307"/>
+      <c r="Q7" s="298"/>
       <c r="R7" s="43" t="s">
         <v>34</v>
       </c>
@@ -12313,9 +12365,9 @@
       <c r="T7" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="U7" s="307"/>
-      <c r="V7" s="303"/>
-      <c r="W7" s="316"/>
+      <c r="U7" s="298"/>
+      <c r="V7" s="316"/>
+      <c r="W7" s="301"/>
       <c r="X7" s="38"/>
       <c r="Y7" s="38"/>
       <c r="Z7" s="38"/>
@@ -12537,14 +12589,14 @@
       <c r="IH7" s="38"/>
       <c r="II7" s="38"/>
     </row>
-    <row r="8" spans="1:243" s="57" customFormat="1" ht="16.5" thickBot="1">
+    <row r="8" spans="1:243" s="57" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="51">
         <v>1</v>
       </c>
-      <c r="B8" s="308">
+      <c r="B8" s="319">
         <v>2</v>
       </c>
-      <c r="C8" s="309"/>
+      <c r="C8" s="320"/>
       <c r="D8" s="51">
         <v>3</v>
       </c>
@@ -12824,12 +12876,12 @@
       <c r="IH8" s="55"/>
       <c r="II8" s="55"/>
     </row>
-    <row r="9" spans="1:243" s="11" customFormat="1" ht="51.75" customHeight="1" thickTop="1">
+    <row r="9" spans="1:243" s="11" customFormat="1" ht="51.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A9" s="44"/>
-      <c r="B9" s="293" t="s">
+      <c r="B9" s="308" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="294"/>
+      <c r="C9" s="309"/>
       <c r="D9" s="45"/>
       <c r="E9" s="46"/>
       <c r="F9" s="47"/>
@@ -13071,7 +13123,7 @@
       <c r="IH9" s="23"/>
       <c r="II9" s="23"/>
     </row>
-    <row r="10" spans="1:243" s="9" customFormat="1" ht="94.5">
+    <row r="10" spans="1:243" s="9" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2" t="s">
         <v>15</v>
@@ -13334,12 +13386,12 @@
       <c r="IH10" s="7"/>
       <c r="II10" s="7"/>
     </row>
-    <row r="11" spans="1:243" s="9" customFormat="1" ht="45.75" customHeight="1">
+    <row r="11" spans="1:243" s="9" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="295" t="s">
+      <c r="B11" s="310" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="296"/>
+      <c r="C11" s="311"/>
       <c r="D11" s="25"/>
       <c r="E11" s="4"/>
       <c r="F11" s="13"/>
@@ -13580,7 +13632,7 @@
       <c r="IH11" s="7"/>
       <c r="II11" s="7"/>
     </row>
-    <row r="12" spans="1:243" s="9" customFormat="1" ht="31.5">
+    <row r="12" spans="1:243" s="9" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="2" t="s">
         <v>18</v>
@@ -13836,7 +13888,7 @@
       <c r="IH12" s="7"/>
       <c r="II12" s="7"/>
     </row>
-    <row r="13" spans="1:243" s="9" customFormat="1" ht="31.5">
+    <row r="13" spans="1:243" s="9" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="C13" s="17"/>
@@ -14088,7 +14140,7 @@
       <c r="IH13" s="7"/>
       <c r="II13" s="7"/>
     </row>
-    <row r="14" spans="1:243" s="34" customFormat="1" ht="16.5" thickBot="1">
+    <row r="14" spans="1:243" s="34" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="26"/>
       <c r="B14" s="27"/>
       <c r="C14" s="28"/>
@@ -14333,7 +14385,7 @@
       <c r="IH14" s="32"/>
       <c r="II14" s="32"/>
     </row>
-    <row r="15" spans="1:243" ht="16.5" thickTop="1">
+    <row r="15" spans="1:243" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A15" s="35"/>
       <c r="B15" s="35"/>
       <c r="C15" s="35"/>
@@ -14341,14 +14393,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B5:C7"/>
-    <mergeCell ref="G5:G7"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="H5:H7"/>
-    <mergeCell ref="W5:W7"/>
-    <mergeCell ref="R5:T5"/>
-    <mergeCell ref="I5:M5"/>
-    <mergeCell ref="M6:M7"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="F5:F7"/>
@@ -14365,8 +14409,16 @@
     <mergeCell ref="Q5:Q7"/>
     <mergeCell ref="U5:U7"/>
     <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B5:C7"/>
+    <mergeCell ref="G5:G7"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="H5:H7"/>
+    <mergeCell ref="W5:W7"/>
+    <mergeCell ref="R5:T5"/>
+    <mergeCell ref="I5:M5"/>
+    <mergeCell ref="M6:M7"/>
   </mergeCells>
   <pageMargins left="0.19" right="0.17" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="56" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
+  <pageSetup paperSize="10001" scale="49" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>